<commit_message>
Task 2 mit Auswertung, aufräumen so dass nur noch 2 py-dateien im Top-Folder da sind.
</commit_message>
<xml_diff>
--- a/Auswertung.xlsx
+++ b/Auswertung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22116" windowHeight="8496"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22116" windowHeight="8496" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="task1result" localSheetId="0">Tabelle1!$A$1:$D$52</definedName>
+    <definedName name="task2result" localSheetId="1">Tabelle2!$A$3:$H$54</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -28,13 +29,49 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="task2result" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\ADM\task2result.csv" decimal="," thousands=" " comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Eventcount</t>
+  </si>
+  <si>
+    <t>Errorcount</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Anz. Res_send</t>
+  </si>
+  <si>
+    <t>Average Duration</t>
+  </si>
+  <si>
+    <t>Anzahl client events</t>
+  </si>
+  <si>
+    <t>Anzahl client Fehler</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -65,9 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -457,11 +495,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="255070208"/>
-        <c:axId val="255071744"/>
+        <c:axId val="243183616"/>
+        <c:axId val="243185152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="255070208"/>
+        <c:axId val="243183616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,7 +509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="255071744"/>
+        <c:crossAx val="243185152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -479,7 +517,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="255071744"/>
+        <c:axId val="243185152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,10 +528,1507 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="255070208"/>
+        <c:crossAx val="243183616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Anzahl Nachrichten &amp; Antworten Client</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle2!$E$2:$E$53</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>41937.640277777777</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41937.640972222223</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41937.64166666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41937.642361111109</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41937.643055555556</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41937.643750000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41937.644444444442</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41937.645138888889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41937.645833333336</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41937.646527777775</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41937.647222222222</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41937.647916666669</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41937.648611111108</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41937.649305555555</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41937.65</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41937.650694444441</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41937.651388888888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41937.652083333334</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41937.652777777781</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41937.65347222222</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41937.654166666667</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41937.654861111114</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41937.655555555553</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41937.65625</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41937.656944444447</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41937.657638888886</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41937.658333333333</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41937.65902777778</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41937.659722222219</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41937.660416666666</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41937.661111111112</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41937.661805555559</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41937.662499999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41937.663194444445</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41937.663888888892</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41937.664583333331</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41937.665277777778</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41937.665972222225</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41937.666666666664</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41937.667361111111</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41937.668055555558</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41937.668749999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41937.669444444444</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>41937.670138888891</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>41937.67083333333</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>41937.671527777777</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>41937.672222222223</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>41937.67291666667</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>41937.673611111109</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>41937.674305555556</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>41937.675000000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>41937.675694444442</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$H$2:$H$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>98686</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86715</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89248</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84445</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80223</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69397</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63450</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56804</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55026</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54119</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52197</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50868</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50053</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>47628</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>46907</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45163</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45294</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44401</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42654</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43153</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41853</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40867</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40644</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39571</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39070</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38358</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37559</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37649</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>37395</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>36968</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>36064</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34169</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34230</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>34507</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>34075</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>34472</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>33341</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>33558</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>33318</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>32923</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>32128</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>31728</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>31055</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>31339</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>31207</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>30777</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>29273</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>27988</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>28168</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>23844</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Anzahl Fehler Client</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle2!$E$2:$E$53</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>41937.640277777777</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41937.640972222223</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41937.64166666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41937.642361111109</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41937.643055555556</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41937.643750000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41937.644444444442</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41937.645138888889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41937.645833333336</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41937.646527777775</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41937.647222222222</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41937.647916666669</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41937.648611111108</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41937.649305555555</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41937.65</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41937.650694444441</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41937.651388888888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41937.652083333334</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41937.652777777781</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41937.65347222222</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41937.654166666667</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41937.654861111114</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41937.655555555553</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41937.65625</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41937.656944444447</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41937.657638888886</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41937.658333333333</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41937.65902777778</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41937.659722222219</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41937.660416666666</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41937.661111111112</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41937.661805555559</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41937.662499999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41937.663194444445</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41937.663888888892</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41937.664583333331</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41937.665277777778</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41937.665972222225</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41937.666666666664</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41937.667361111111</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41937.668055555558</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41937.668749999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41937.669444444444</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>41937.670138888891</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>41937.67083333333</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>41937.671527777777</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>41937.672222222223</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>41937.67291666667</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>41937.673611111109</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>41937.674305555556</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>41937.675000000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>41937.675694444442</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$I$2:$I$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>33366</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30183</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32545</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32933</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32814</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31620</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30257</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27481</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25055</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24247</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23873</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23346</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22616</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22196</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21171</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20731</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20153</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20267</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19842</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18841</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18990</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>18519</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18297</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17905</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>17851</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>17418</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>16993</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>16635</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>16288</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>16335</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>16061</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15884</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15748</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>14650</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>14631</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>14749</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14486</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14899</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>14088</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>14120</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>14225</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14068</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>13558</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>13324</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>13042</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>13004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>12951</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>12941</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12187</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>11418</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>11706</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>9737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Anzahl res_send Server</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle2!$E$2:$E$53</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>41937.640277777777</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41937.640972222223</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41937.64166666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41937.642361111109</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41937.643055555556</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41937.643750000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41937.644444444442</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41937.645138888889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41937.645833333336</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41937.646527777775</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41937.647222222222</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41937.647916666669</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41937.648611111108</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41937.649305555555</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41937.65</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41937.650694444441</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41937.651388888888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41937.652083333334</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41937.652777777781</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41937.65347222222</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41937.654166666667</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41937.654861111114</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41937.655555555553</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41937.65625</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41937.656944444447</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41937.657638888886</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41937.658333333333</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41937.65902777778</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41937.659722222219</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41937.660416666666</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41937.661111111112</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41937.661805555559</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41937.662499999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41937.663194444445</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41937.663888888892</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41937.664583333331</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41937.665277777778</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41937.665972222225</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41937.666666666664</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41937.667361111111</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41937.668055555558</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41937.668749999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41937.669444444444</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>41937.670138888891</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>41937.67083333333</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>41937.671527777777</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>41937.672222222223</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>41937.67291666667</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>41937.673611111109</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>41937.674305555556</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>41937.675000000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>41937.675694444442</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$F$2:$F$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>25669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22612</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23366</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21049</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19422</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16722</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14897</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14461</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14214</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13707</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13431</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13228</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12647</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12479</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12028</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12043</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11723</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11232</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11341</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11029</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11030</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10764</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10815</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10390</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10292</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10189</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9877</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10010</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9805</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9768</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9556</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8995</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9151</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9032</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8819</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8755</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8707</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8687</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8458</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8463</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8218</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8374</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8261</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8096</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>11708</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>14966</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>15136</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>18247</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="141383936"/>
+        <c:axId val="142508032"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Durchschnittliche Dauer (Sekunden)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle2!$E$2:$E$53</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>41937.640277777777</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41937.640972222223</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41937.64166666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41937.642361111109</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41937.643055555556</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41937.643750000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41937.644444444442</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41937.645138888889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41937.645833333336</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41937.646527777775</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41937.647222222222</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41937.647916666669</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41937.648611111108</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41937.649305555555</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41937.65</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41937.650694444441</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41937.651388888888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41937.652083333334</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41937.652777777781</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41937.65347222222</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41937.654166666667</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41937.654861111114</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41937.655555555553</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41937.65625</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41937.656944444447</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41937.657638888886</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41937.658333333333</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41937.65902777778</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41937.659722222219</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41937.660416666666</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41937.661111111112</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41937.661805555559</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41937.662499999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41937.663194444445</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41937.663888888892</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41937.664583333331</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41937.665277777778</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41937.665972222225</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41937.666666666664</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41937.667361111111</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41937.668055555558</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41937.668749999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41937.669444444444</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>41937.670138888891</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>41937.67083333333</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>41937.671527777777</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>41937.672222222223</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>41937.67291666667</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>41937.673611111109</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>41937.674305555556</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>41937.675000000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>41937.675694444442</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$G$2:$G$53</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>24.5604746367265</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.4735512887043</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.560494352814601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.350843744449001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.103336948256697</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.022887989203703</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.577719497960999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44.420677698975503</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>49.579994366593901</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51.189637625849599</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.065780964171502</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>53.983121635342997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55.412793897931898</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>56.267816114918098</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>59.185815066767397</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>60.022043618223201</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>62.395655735889903</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>62.214995363624297</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>63.424607553883902</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>66.064495709663802</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>65.271383217852701</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>67.253996659508402</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>67.301913841301698</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>68.947488193407807</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>69.278909556146004</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>71.233959212554595</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>72.083823905809993</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>73.450701287866906</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>75.017625602385493</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>74.884299715795905</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>75.3307394036635</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>76.205096299502202</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>78.113880878438295</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>82.531505165500803</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>82.278410750803303</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>81.690236763555205</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>82.642553191489299</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>81.772075887676905</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>84.482169101106706</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>84.006794207044507</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>84.517107869620006</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>85.642924399356005</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>87.626929780876495</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>88.971570852244</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>90.647721783931701</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>89.903793994702994</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>90.415836190598199</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>89.568963836631198</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>61.676630341953299</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>51.428112048020502</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50.955232888383897</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>36.352583459151099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="307723648"/>
+        <c:axId val="307720576"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="141383936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="142508032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="142508032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141383936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="307720576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="307723648"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="307723648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="307720576"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -547,8 +2082,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Diagramm 16"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="task1result" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="task2result" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -840,8 +2414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1483,13 +3057,1456 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E2" s="1">
+        <f>(((A3)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.640277777777</v>
+      </c>
+      <c r="F2">
+        <v>25669</v>
+      </c>
+      <c r="G2" s="2">
+        <v>24.5604746367265</v>
+      </c>
+      <c r="H2">
+        <v>98686</v>
+      </c>
+      <c r="I2">
+        <v>33366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>23570842</v>
+      </c>
+      <c r="B3">
+        <v>98686</v>
+      </c>
+      <c r="C3">
+        <v>33366</v>
+      </c>
+      <c r="E3" s="1">
+        <f>(((A4)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.640972222223</v>
+      </c>
+      <c r="F3">
+        <v>22612</v>
+      </c>
+      <c r="G3" s="2">
+        <v>32.4735512887043</v>
+      </c>
+      <c r="H3">
+        <v>86715</v>
+      </c>
+      <c r="I3">
+        <v>30183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>23570843</v>
+      </c>
+      <c r="B4">
+        <v>86715</v>
+      </c>
+      <c r="C4">
+        <v>30183</v>
+      </c>
+      <c r="E4" s="1">
+        <f>(((A5)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.64166666667</v>
+      </c>
+      <c r="F4">
+        <v>23366</v>
+      </c>
+      <c r="G4" s="2">
+        <v>31.560494352814601</v>
+      </c>
+      <c r="H4">
+        <v>89248</v>
+      </c>
+      <c r="I4">
+        <v>32545</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>23570844</v>
+      </c>
+      <c r="B5">
+        <v>89248</v>
+      </c>
+      <c r="C5">
+        <v>32545</v>
+      </c>
+      <c r="E5" s="1">
+        <f>(((A6)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.642361111109</v>
+      </c>
+      <c r="F5">
+        <v>22102</v>
+      </c>
+      <c r="G5" s="2">
+        <v>33.350843744449001</v>
+      </c>
+      <c r="H5">
+        <v>84445</v>
+      </c>
+      <c r="I5">
+        <v>32933</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>23570845</v>
+      </c>
+      <c r="B6">
+        <v>84445</v>
+      </c>
+      <c r="C6">
+        <v>32933</v>
+      </c>
+      <c r="E6" s="1">
+        <f>(((A7)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.643055555556</v>
+      </c>
+      <c r="F6">
+        <v>21049</v>
+      </c>
+      <c r="G6" s="2">
+        <v>35.103336948256697</v>
+      </c>
+      <c r="H6">
+        <v>80223</v>
+      </c>
+      <c r="I6">
+        <v>32814</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>23570846</v>
+      </c>
+      <c r="B7">
+        <v>80223</v>
+      </c>
+      <c r="C7">
+        <v>32814</v>
+      </c>
+      <c r="E7" s="1">
+        <f>(((A8)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.643750000003</v>
+      </c>
+      <c r="F7">
+        <v>19422</v>
+      </c>
+      <c r="G7" s="2">
+        <v>38.022887989203703</v>
+      </c>
+      <c r="H7">
+        <v>74100</v>
+      </c>
+      <c r="I7">
+        <v>31620</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>23570847</v>
+      </c>
+      <c r="B8">
+        <v>74100</v>
+      </c>
+      <c r="C8">
+        <v>31620</v>
+      </c>
+      <c r="E8" s="1">
+        <f>(((A9)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.644444444442</v>
+      </c>
+      <c r="F8">
+        <v>18125</v>
+      </c>
+      <c r="G8" s="2">
+        <v>40.577719497960999</v>
+      </c>
+      <c r="H8">
+        <v>69397</v>
+      </c>
+      <c r="I8">
+        <v>30257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>23570848</v>
+      </c>
+      <c r="B9">
+        <v>69397</v>
+      </c>
+      <c r="C9">
+        <v>30257</v>
+      </c>
+      <c r="E9" s="1">
+        <f>(((A10)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.645138888889</v>
+      </c>
+      <c r="F9">
+        <v>16722</v>
+      </c>
+      <c r="G9" s="2">
+        <v>44.420677698975503</v>
+      </c>
+      <c r="H9">
+        <v>63450</v>
+      </c>
+      <c r="I9">
+        <v>27481</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>23570849</v>
+      </c>
+      <c r="B10">
+        <v>63450</v>
+      </c>
+      <c r="C10">
+        <v>27481</v>
+      </c>
+      <c r="E10" s="1">
+        <f>(((A11)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.645833333336</v>
+      </c>
+      <c r="F10">
+        <v>14897</v>
+      </c>
+      <c r="G10" s="2">
+        <v>49.579994366593901</v>
+      </c>
+      <c r="H10">
+        <v>56804</v>
+      </c>
+      <c r="I10">
+        <v>25055</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>23570850</v>
+      </c>
+      <c r="B11">
+        <v>56804</v>
+      </c>
+      <c r="C11">
+        <v>25055</v>
+      </c>
+      <c r="E11" s="1">
+        <f>(((A12)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.646527777775</v>
+      </c>
+      <c r="F11">
+        <v>14461</v>
+      </c>
+      <c r="G11" s="2">
+        <v>51.189637625849599</v>
+      </c>
+      <c r="H11">
+        <v>55026</v>
+      </c>
+      <c r="I11">
+        <v>24247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>23570851</v>
+      </c>
+      <c r="B12">
+        <v>55026</v>
+      </c>
+      <c r="C12">
+        <v>24247</v>
+      </c>
+      <c r="E12" s="1">
+        <f>(((A13)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.647222222222</v>
+      </c>
+      <c r="F12">
+        <v>14214</v>
+      </c>
+      <c r="G12" s="2">
+        <v>52.065780964171502</v>
+      </c>
+      <c r="H12">
+        <v>54119</v>
+      </c>
+      <c r="I12">
+        <v>23873</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>23570852</v>
+      </c>
+      <c r="B13">
+        <v>54119</v>
+      </c>
+      <c r="C13">
+        <v>23873</v>
+      </c>
+      <c r="E13" s="1">
+        <f>(((A14)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.647916666669</v>
+      </c>
+      <c r="F13">
+        <v>13707</v>
+      </c>
+      <c r="G13" s="2">
+        <v>53.983121635342997</v>
+      </c>
+      <c r="H13">
+        <v>52197</v>
+      </c>
+      <c r="I13">
+        <v>23346</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>23570853</v>
+      </c>
+      <c r="B14">
+        <v>52197</v>
+      </c>
+      <c r="C14">
+        <v>23346</v>
+      </c>
+      <c r="E14" s="1">
+        <f>(((A15)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.648611111108</v>
+      </c>
+      <c r="F14">
+        <v>13431</v>
+      </c>
+      <c r="G14" s="2">
+        <v>55.412793897931898</v>
+      </c>
+      <c r="H14">
+        <v>50868</v>
+      </c>
+      <c r="I14">
+        <v>22616</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>23570854</v>
+      </c>
+      <c r="B15">
+        <v>50868</v>
+      </c>
+      <c r="C15">
+        <v>22616</v>
+      </c>
+      <c r="E15" s="1">
+        <f>(((A16)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.649305555555</v>
+      </c>
+      <c r="F15">
+        <v>13228</v>
+      </c>
+      <c r="G15" s="2">
+        <v>56.267816114918098</v>
+      </c>
+      <c r="H15">
+        <v>50053</v>
+      </c>
+      <c r="I15">
+        <v>22196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>23570855</v>
+      </c>
+      <c r="B16">
+        <v>50053</v>
+      </c>
+      <c r="C16">
+        <v>22196</v>
+      </c>
+      <c r="E16" s="1">
+        <f>(((A17)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.65</v>
+      </c>
+      <c r="F16">
+        <v>12647</v>
+      </c>
+      <c r="G16" s="2">
+        <v>59.185815066767397</v>
+      </c>
+      <c r="H16">
+        <v>47628</v>
+      </c>
+      <c r="I16">
+        <v>21171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>23570856</v>
+      </c>
+      <c r="B17">
+        <v>47628</v>
+      </c>
+      <c r="C17">
+        <v>21171</v>
+      </c>
+      <c r="E17" s="1">
+        <f>(((A18)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.650694444441</v>
+      </c>
+      <c r="F17">
+        <v>12479</v>
+      </c>
+      <c r="G17" s="2">
+        <v>60.022043618223201</v>
+      </c>
+      <c r="H17">
+        <v>46907</v>
+      </c>
+      <c r="I17">
+        <v>20731</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>23570857</v>
+      </c>
+      <c r="B18">
+        <v>46907</v>
+      </c>
+      <c r="C18">
+        <v>20731</v>
+      </c>
+      <c r="E18" s="1">
+        <f>(((A19)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.651388888888</v>
+      </c>
+      <c r="F18">
+        <v>12028</v>
+      </c>
+      <c r="G18" s="2">
+        <v>62.395655735889903</v>
+      </c>
+      <c r="H18">
+        <v>45163</v>
+      </c>
+      <c r="I18">
+        <v>20153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>23570858</v>
+      </c>
+      <c r="B19">
+        <v>45163</v>
+      </c>
+      <c r="C19">
+        <v>20153</v>
+      </c>
+      <c r="E19" s="1">
+        <f>(((A20)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.652083333334</v>
+      </c>
+      <c r="F19">
+        <v>12043</v>
+      </c>
+      <c r="G19" s="2">
+        <v>62.214995363624297</v>
+      </c>
+      <c r="H19">
+        <v>45294</v>
+      </c>
+      <c r="I19">
+        <v>20267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>23570859</v>
+      </c>
+      <c r="B20">
+        <v>45294</v>
+      </c>
+      <c r="C20">
+        <v>20267</v>
+      </c>
+      <c r="E20" s="1">
+        <f>(((A21)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.652777777781</v>
+      </c>
+      <c r="F20">
+        <v>11723</v>
+      </c>
+      <c r="G20" s="2">
+        <v>63.424607553883902</v>
+      </c>
+      <c r="H20">
+        <v>44401</v>
+      </c>
+      <c r="I20">
+        <v>19842</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>23570860</v>
+      </c>
+      <c r="B21">
+        <v>44401</v>
+      </c>
+      <c r="C21">
+        <v>19842</v>
+      </c>
+      <c r="E21" s="1">
+        <f>(((A22)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.65347222222</v>
+      </c>
+      <c r="F21">
+        <v>11232</v>
+      </c>
+      <c r="G21" s="2">
+        <v>66.064495709663802</v>
+      </c>
+      <c r="H21">
+        <v>42654</v>
+      </c>
+      <c r="I21">
+        <v>18841</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>23570861</v>
+      </c>
+      <c r="B22">
+        <v>42654</v>
+      </c>
+      <c r="C22">
+        <v>18841</v>
+      </c>
+      <c r="E22" s="1">
+        <f>(((A23)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.654166666667</v>
+      </c>
+      <c r="F22">
+        <v>11341</v>
+      </c>
+      <c r="G22" s="2">
+        <v>65.271383217852701</v>
+      </c>
+      <c r="H22">
+        <v>43153</v>
+      </c>
+      <c r="I22">
+        <v>18990</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>23570862</v>
+      </c>
+      <c r="B23">
+        <v>43153</v>
+      </c>
+      <c r="C23">
+        <v>18990</v>
+      </c>
+      <c r="E23" s="1">
+        <f>(((A24)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.654861111114</v>
+      </c>
+      <c r="F23">
+        <v>11029</v>
+      </c>
+      <c r="G23" s="2">
+        <v>67.253996659508402</v>
+      </c>
+      <c r="H23">
+        <v>41910</v>
+      </c>
+      <c r="I23">
+        <v>18519</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23570863</v>
+      </c>
+      <c r="B24">
+        <v>41910</v>
+      </c>
+      <c r="C24">
+        <v>18519</v>
+      </c>
+      <c r="E24" s="1">
+        <f>(((A25)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.655555555553</v>
+      </c>
+      <c r="F24">
+        <v>11030</v>
+      </c>
+      <c r="G24" s="2">
+        <v>67.301913841301698</v>
+      </c>
+      <c r="H24">
+        <v>41853</v>
+      </c>
+      <c r="I24">
+        <v>18297</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23570864</v>
+      </c>
+      <c r="B25">
+        <v>41853</v>
+      </c>
+      <c r="C25">
+        <v>18297</v>
+      </c>
+      <c r="E25" s="1">
+        <f>(((A26)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.65625</v>
+      </c>
+      <c r="F25">
+        <v>10764</v>
+      </c>
+      <c r="G25" s="2">
+        <v>68.947488193407807</v>
+      </c>
+      <c r="H25">
+        <v>40867</v>
+      </c>
+      <c r="I25">
+        <v>17905</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>23570865</v>
+      </c>
+      <c r="B26">
+        <v>40867</v>
+      </c>
+      <c r="C26">
+        <v>17905</v>
+      </c>
+      <c r="E26" s="1">
+        <f>(((A27)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.656944444447</v>
+      </c>
+      <c r="F26">
+        <v>10815</v>
+      </c>
+      <c r="G26" s="2">
+        <v>69.278909556146004</v>
+      </c>
+      <c r="H26">
+        <v>40644</v>
+      </c>
+      <c r="I26">
+        <v>17851</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>23570866</v>
+      </c>
+      <c r="B27">
+        <v>40644</v>
+      </c>
+      <c r="C27">
+        <v>17851</v>
+      </c>
+      <c r="E27" s="1">
+        <f>(((A28)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.657638888886</v>
+      </c>
+      <c r="F27">
+        <v>10390</v>
+      </c>
+      <c r="G27" s="2">
+        <v>71.233959212554595</v>
+      </c>
+      <c r="H27">
+        <v>39571</v>
+      </c>
+      <c r="I27">
+        <v>17418</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>23570867</v>
+      </c>
+      <c r="B28">
+        <v>39571</v>
+      </c>
+      <c r="C28">
+        <v>17418</v>
+      </c>
+      <c r="E28" s="1">
+        <f>(((A29)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.658333333333</v>
+      </c>
+      <c r="F28">
+        <v>10292</v>
+      </c>
+      <c r="G28" s="2">
+        <v>72.083823905809993</v>
+      </c>
+      <c r="H28">
+        <v>39070</v>
+      </c>
+      <c r="I28">
+        <v>16993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>23570868</v>
+      </c>
+      <c r="B29">
+        <v>39070</v>
+      </c>
+      <c r="C29">
+        <v>16993</v>
+      </c>
+      <c r="E29" s="1">
+        <f>(((A30)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.65902777778</v>
+      </c>
+      <c r="F29">
+        <v>10189</v>
+      </c>
+      <c r="G29" s="2">
+        <v>73.450701287866906</v>
+      </c>
+      <c r="H29">
+        <v>38358</v>
+      </c>
+      <c r="I29">
+        <v>16635</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>23570869</v>
+      </c>
+      <c r="B30">
+        <v>38358</v>
+      </c>
+      <c r="C30">
+        <v>16635</v>
+      </c>
+      <c r="E30" s="1">
+        <f>(((A31)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.659722222219</v>
+      </c>
+      <c r="F30">
+        <v>9877</v>
+      </c>
+      <c r="G30" s="2">
+        <v>75.017625602385493</v>
+      </c>
+      <c r="H30">
+        <v>37559</v>
+      </c>
+      <c r="I30">
+        <v>16288</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>23570870</v>
+      </c>
+      <c r="B31">
+        <v>37559</v>
+      </c>
+      <c r="C31">
+        <v>16288</v>
+      </c>
+      <c r="E31" s="1">
+        <f>(((A32)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.660416666666</v>
+      </c>
+      <c r="F31">
+        <v>10010</v>
+      </c>
+      <c r="G31" s="2">
+        <v>74.884299715795905</v>
+      </c>
+      <c r="H31">
+        <v>37649</v>
+      </c>
+      <c r="I31">
+        <v>16335</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>23570871</v>
+      </c>
+      <c r="B32">
+        <v>37649</v>
+      </c>
+      <c r="C32">
+        <v>16335</v>
+      </c>
+      <c r="E32" s="1">
+        <f>(((A33)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.661111111112</v>
+      </c>
+      <c r="F32">
+        <v>9805</v>
+      </c>
+      <c r="G32" s="2">
+        <v>75.3307394036635</v>
+      </c>
+      <c r="H32">
+        <v>37395</v>
+      </c>
+      <c r="I32">
+        <v>16061</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>23570872</v>
+      </c>
+      <c r="B33">
+        <v>37395</v>
+      </c>
+      <c r="C33">
+        <v>16061</v>
+      </c>
+      <c r="E33" s="1">
+        <f>(((A34)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.661805555559</v>
+      </c>
+      <c r="F33">
+        <v>9768</v>
+      </c>
+      <c r="G33" s="2">
+        <v>76.205096299502202</v>
+      </c>
+      <c r="H33">
+        <v>36968</v>
+      </c>
+      <c r="I33">
+        <v>15884</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>23570873</v>
+      </c>
+      <c r="B34">
+        <v>36968</v>
+      </c>
+      <c r="C34">
+        <v>15884</v>
+      </c>
+      <c r="E34" s="1">
+        <f>(((A35)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.662499999999</v>
+      </c>
+      <c r="F34">
+        <v>9556</v>
+      </c>
+      <c r="G34" s="2">
+        <v>78.113880878438295</v>
+      </c>
+      <c r="H34">
+        <v>36064</v>
+      </c>
+      <c r="I34">
+        <v>15748</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>23570874</v>
+      </c>
+      <c r="B35">
+        <v>36064</v>
+      </c>
+      <c r="C35">
+        <v>15748</v>
+      </c>
+      <c r="E35" s="1">
+        <f>(((A36)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.663194444445</v>
+      </c>
+      <c r="F35">
+        <v>8995</v>
+      </c>
+      <c r="G35" s="2">
+        <v>82.531505165500803</v>
+      </c>
+      <c r="H35">
+        <v>34169</v>
+      </c>
+      <c r="I35">
+        <v>14650</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>23570875</v>
+      </c>
+      <c r="B36">
+        <v>34169</v>
+      </c>
+      <c r="C36">
+        <v>14650</v>
+      </c>
+      <c r="E36" s="1">
+        <f>(((A37)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.663888888892</v>
+      </c>
+      <c r="F36">
+        <v>9002</v>
+      </c>
+      <c r="G36" s="2">
+        <v>82.278410750803303</v>
+      </c>
+      <c r="H36">
+        <v>34230</v>
+      </c>
+      <c r="I36">
+        <v>14631</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>23570876</v>
+      </c>
+      <c r="B37">
+        <v>34230</v>
+      </c>
+      <c r="C37">
+        <v>14631</v>
+      </c>
+      <c r="E37" s="1">
+        <f>(((A38)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.664583333331</v>
+      </c>
+      <c r="F37">
+        <v>9151</v>
+      </c>
+      <c r="G37" s="2">
+        <v>81.690236763555205</v>
+      </c>
+      <c r="H37">
+        <v>34507</v>
+      </c>
+      <c r="I37">
+        <v>14749</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>23570877</v>
+      </c>
+      <c r="B38">
+        <v>34507</v>
+      </c>
+      <c r="C38">
+        <v>14749</v>
+      </c>
+      <c r="E38" s="1">
+        <f>(((A39)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.665277777778</v>
+      </c>
+      <c r="F38">
+        <v>8995</v>
+      </c>
+      <c r="G38" s="2">
+        <v>82.642553191489299</v>
+      </c>
+      <c r="H38">
+        <v>34075</v>
+      </c>
+      <c r="I38">
+        <v>14486</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>23570878</v>
+      </c>
+      <c r="B39">
+        <v>34075</v>
+      </c>
+      <c r="C39">
+        <v>14486</v>
+      </c>
+      <c r="E39" s="1">
+        <f>(((A40)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.665972222225</v>
+      </c>
+      <c r="F39">
+        <v>9032</v>
+      </c>
+      <c r="G39" s="2">
+        <v>81.772075887676905</v>
+      </c>
+      <c r="H39">
+        <v>34472</v>
+      </c>
+      <c r="I39">
+        <v>14899</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>23570879</v>
+      </c>
+      <c r="B40">
+        <v>34472</v>
+      </c>
+      <c r="C40">
+        <v>14899</v>
+      </c>
+      <c r="E40" s="1">
+        <f>(((A41)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.666666666664</v>
+      </c>
+      <c r="F40">
+        <v>8819</v>
+      </c>
+      <c r="G40" s="2">
+        <v>84.482169101106706</v>
+      </c>
+      <c r="H40">
+        <v>33341</v>
+      </c>
+      <c r="I40">
+        <v>14088</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>23570880</v>
+      </c>
+      <c r="B41">
+        <v>33341</v>
+      </c>
+      <c r="C41">
+        <v>14088</v>
+      </c>
+      <c r="E41" s="1">
+        <f>(((A42)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.667361111111</v>
+      </c>
+      <c r="F41">
+        <v>8755</v>
+      </c>
+      <c r="G41" s="2">
+        <v>84.006794207044507</v>
+      </c>
+      <c r="H41">
+        <v>33558</v>
+      </c>
+      <c r="I41">
+        <v>14120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>23570881</v>
+      </c>
+      <c r="B42">
+        <v>33558</v>
+      </c>
+      <c r="C42">
+        <v>14120</v>
+      </c>
+      <c r="E42" s="1">
+        <f>(((A43)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.668055555558</v>
+      </c>
+      <c r="F42">
+        <v>8707</v>
+      </c>
+      <c r="G42" s="2">
+        <v>84.517107869620006</v>
+      </c>
+      <c r="H42">
+        <v>33318</v>
+      </c>
+      <c r="I42">
+        <v>14225</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>23570882</v>
+      </c>
+      <c r="B43">
+        <v>33318</v>
+      </c>
+      <c r="C43">
+        <v>14225</v>
+      </c>
+      <c r="E43" s="1">
+        <f>(((A44)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.668749999997</v>
+      </c>
+      <c r="F43">
+        <v>8687</v>
+      </c>
+      <c r="G43" s="2">
+        <v>85.642924399356005</v>
+      </c>
+      <c r="H43">
+        <v>32923</v>
+      </c>
+      <c r="I43">
+        <v>14068</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>23570883</v>
+      </c>
+      <c r="B44">
+        <v>32923</v>
+      </c>
+      <c r="C44">
+        <v>14068</v>
+      </c>
+      <c r="E44" s="1">
+        <f>(((A45)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.669444444444</v>
+      </c>
+      <c r="F44">
+        <v>8458</v>
+      </c>
+      <c r="G44" s="2">
+        <v>87.626929780876495</v>
+      </c>
+      <c r="H44">
+        <v>32128</v>
+      </c>
+      <c r="I44">
+        <v>13558</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>23570884</v>
+      </c>
+      <c r="B45">
+        <v>32128</v>
+      </c>
+      <c r="C45">
+        <v>13558</v>
+      </c>
+      <c r="E45" s="1">
+        <f>(((A46)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.670138888891</v>
+      </c>
+      <c r="F45">
+        <v>8463</v>
+      </c>
+      <c r="G45" s="2">
+        <v>88.971570852244</v>
+      </c>
+      <c r="H45">
+        <v>31728</v>
+      </c>
+      <c r="I45">
+        <v>13324</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>23570885</v>
+      </c>
+      <c r="B46">
+        <v>31728</v>
+      </c>
+      <c r="C46">
+        <v>13324</v>
+      </c>
+      <c r="E46" s="1">
+        <f>(((A47)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.67083333333</v>
+      </c>
+      <c r="F46">
+        <v>8218</v>
+      </c>
+      <c r="G46" s="2">
+        <v>90.647721783931701</v>
+      </c>
+      <c r="H46">
+        <v>31055</v>
+      </c>
+      <c r="I46">
+        <v>13042</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>23570886</v>
+      </c>
+      <c r="B47">
+        <v>31055</v>
+      </c>
+      <c r="C47">
+        <v>13042</v>
+      </c>
+      <c r="E47" s="1">
+        <f>(((A48)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.671527777777</v>
+      </c>
+      <c r="F47">
+        <v>8374</v>
+      </c>
+      <c r="G47" s="2">
+        <v>89.903793994702994</v>
+      </c>
+      <c r="H47">
+        <v>31339</v>
+      </c>
+      <c r="I47">
+        <v>13004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>23570887</v>
+      </c>
+      <c r="B48">
+        <v>31339</v>
+      </c>
+      <c r="C48">
+        <v>13004</v>
+      </c>
+      <c r="E48" s="1">
+        <f>(((A49)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.672222222223</v>
+      </c>
+      <c r="F48">
+        <v>8261</v>
+      </c>
+      <c r="G48" s="2">
+        <v>90.415836190598199</v>
+      </c>
+      <c r="H48">
+        <v>31207</v>
+      </c>
+      <c r="I48">
+        <v>12951</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>23570888</v>
+      </c>
+      <c r="B49">
+        <v>31207</v>
+      </c>
+      <c r="C49">
+        <v>12951</v>
+      </c>
+      <c r="E49" s="1">
+        <f>(((A50)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.67291666667</v>
+      </c>
+      <c r="F49">
+        <v>8096</v>
+      </c>
+      <c r="G49" s="2">
+        <v>89.568963836631198</v>
+      </c>
+      <c r="H49">
+        <v>30777</v>
+      </c>
+      <c r="I49">
+        <v>12941</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>23570889</v>
+      </c>
+      <c r="B50">
+        <v>30777</v>
+      </c>
+      <c r="C50">
+        <v>12941</v>
+      </c>
+      <c r="E50" s="1">
+        <f>(((A51)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.673611111109</v>
+      </c>
+      <c r="F50">
+        <v>11708</v>
+      </c>
+      <c r="G50" s="2">
+        <v>61.676630341953299</v>
+      </c>
+      <c r="H50">
+        <v>29273</v>
+      </c>
+      <c r="I50">
+        <v>12187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>23570890</v>
+      </c>
+      <c r="B51">
+        <v>29273</v>
+      </c>
+      <c r="C51">
+        <v>12187</v>
+      </c>
+      <c r="E51" s="1">
+        <f>(((A52)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.674305555556</v>
+      </c>
+      <c r="F51">
+        <v>14966</v>
+      </c>
+      <c r="G51" s="2">
+        <v>51.428112048020502</v>
+      </c>
+      <c r="H51">
+        <v>27988</v>
+      </c>
+      <c r="I51">
+        <v>11418</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>23570891</v>
+      </c>
+      <c r="B52">
+        <v>27988</v>
+      </c>
+      <c r="C52">
+        <v>11418</v>
+      </c>
+      <c r="E52" s="1">
+        <f>(((A53)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.675000000003</v>
+      </c>
+      <c r="F52">
+        <v>15136</v>
+      </c>
+      <c r="G52" s="2">
+        <v>50.955232888383897</v>
+      </c>
+      <c r="H52">
+        <v>28168</v>
+      </c>
+      <c r="I52">
+        <v>11706</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>23570892</v>
+      </c>
+      <c r="B53">
+        <v>28168</v>
+      </c>
+      <c r="C53">
+        <v>11706</v>
+      </c>
+      <c r="E53" s="1">
+        <f>(((A54)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.675694444442</v>
+      </c>
+      <c r="F53">
+        <v>18247</v>
+      </c>
+      <c r="G53" s="2">
+        <v>36.352583459151099</v>
+      </c>
+      <c r="H53">
+        <v>23844</v>
+      </c>
+      <c r="I53">
+        <v>9737</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>23570893</v>
+      </c>
+      <c r="B54">
+        <v>23844</v>
+      </c>
+      <c r="C54">
+        <v>9737</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
kommentiert, auswertung schöner formatiert, Durchschnittliche Dauer eines client requests berechnet
</commit_message>
<xml_diff>
--- a/Auswertung.xlsx
+++ b/Auswertung.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="task1result" localSheetId="0">Tabelle1!$A$1:$D$52</definedName>
-    <definedName name="task2result" localSheetId="1">Tabelle2!$A$3:$H$54</definedName>
+    <definedName name="task2result" localSheetId="1">Tabelle2!$A$2:$H$53</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -43,13 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Eventcount</t>
-  </si>
-  <si>
-    <t>Errorcount</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Time</t>
   </si>
@@ -64,6 +58,21 @@
   </si>
   <si>
     <t>Anzahl client Fehler</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dauer pro Minute in Sekunden Average * Anz. Events </t>
+  </si>
+  <si>
+    <t>Dauer pro Minute in Sekunden sum(durations)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Durchschnittliche Dauer eine Client-Requests:</t>
   </si>
 </sst>
 </file>
@@ -135,7 +144,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -495,11 +503,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="243183616"/>
-        <c:axId val="243185152"/>
+        <c:axId val="230764544"/>
+        <c:axId val="230766080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243183616"/>
+        <c:axId val="230764544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,7 +517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243185152"/>
+        <c:crossAx val="230766080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -517,7 +525,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243185152"/>
+        <c:axId val="230766080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,14 +536,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243183616"/>
+        <c:crossAx val="230764544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -581,7 +588,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle2!$E$2:$E$53</c:f>
+              <c:f>Tabelle2!$B$2:$B$53</c:f>
               <c:numCache>
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="52"/>
@@ -746,7 +753,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$H$2:$H$53</c:f>
+              <c:f>Tabelle2!$E$2:$E$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
@@ -922,7 +929,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle2!$E$2:$E$53</c:f>
+              <c:f>Tabelle2!$B$2:$B$53</c:f>
               <c:numCache>
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="52"/>
@@ -1087,7 +1094,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$I$2:$I$53</c:f>
+              <c:f>Tabelle2!$F$2:$F$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
@@ -1263,7 +1270,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle2!$E$2:$E$53</c:f>
+              <c:f>Tabelle2!$B$2:$B$53</c:f>
               <c:numCache>
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="52"/>
@@ -1428,7 +1435,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$F$2:$F$53</c:f>
+              <c:f>Tabelle2!$C$2:$C$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
@@ -1603,8 +1610,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="141383936"/>
-        <c:axId val="142508032"/>
+        <c:axId val="231446400"/>
+        <c:axId val="231447936"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1620,7 +1627,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle2!$E$2:$E$53</c:f>
+              <c:f>Tabelle2!$B$2:$B$53</c:f>
               <c:numCache>
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="52"/>
@@ -1785,7 +1792,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$G$2:$G$53</c:f>
+              <c:f>Tabelle2!$D$2:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="52"/>
@@ -1960,11 +1967,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="307723648"/>
-        <c:axId val="307720576"/>
+        <c:axId val="231459456"/>
+        <c:axId val="231457920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141383936"/>
+        <c:axId val="231446400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1974,7 +1981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142508032"/>
+        <c:crossAx val="231447936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1982,7 +1989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142508032"/>
+        <c:axId val="231447936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1993,12 +2000,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141383936"/>
+        <c:crossAx val="231446400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="307720576"/>
+        <c:axId val="231457920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2008,12 +2015,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="307723648"/>
+        <c:crossAx val="231459456"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="307723648"/>
+        <c:axId val="231459456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2023,7 +2030,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="307720576"/>
+        <c:crossAx val="231457920"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2086,16 +2094,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3057,1450 +3065,1540 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.77734375" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E2" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>23570842</v>
+      </c>
+      <c r="B2" s="1">
+        <f>(((A2)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.640277777777</v>
+      </c>
+      <c r="C2">
+        <v>25669</v>
+      </c>
+      <c r="D2" s="2">
+        <v>24.5604746367265</v>
+      </c>
+      <c r="E2">
+        <v>98686</v>
+      </c>
+      <c r="F2">
+        <v>33366</v>
+      </c>
+      <c r="G2">
+        <f>D2*E2</f>
+        <v>2423774.9999999916</v>
+      </c>
+      <c r="H2">
+        <v>2423775</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>23570843</v>
+      </c>
+      <c r="B3" s="1">
         <f>(((A3)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.640277777777</v>
-      </c>
-      <c r="F2">
-        <v>25669</v>
-      </c>
-      <c r="G2" s="2">
-        <v>24.5604746367265</v>
-      </c>
-      <c r="H2">
-        <v>98686</v>
-      </c>
-      <c r="I2">
-        <v>33366</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>23570842</v>
-      </c>
-      <c r="B3">
-        <v>98686</v>
+        <v>41937.640972222223</v>
       </c>
       <c r="C3">
-        <v>33366</v>
-      </c>
-      <c r="E3" s="1">
+        <v>22612</v>
+      </c>
+      <c r="D3" s="2">
+        <v>32.4735512887043</v>
+      </c>
+      <c r="E3">
+        <v>86715</v>
+      </c>
+      <c r="F3">
+        <v>30183</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G53" si="0">D3*E3</f>
+        <v>2815943.9999999935</v>
+      </c>
+      <c r="H3">
+        <v>2815944</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>23570844</v>
+      </c>
+      <c r="B4" s="1">
         <f>(((A4)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.640972222223</v>
-      </c>
-      <c r="F3">
-        <v>22612</v>
-      </c>
-      <c r="G3" s="2">
-        <v>32.4735512887043</v>
-      </c>
-      <c r="H3">
-        <v>86715</v>
-      </c>
-      <c r="I3">
-        <v>30183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>23570843</v>
-      </c>
-      <c r="B4">
-        <v>86715</v>
+        <v>41937.64166666667</v>
       </c>
       <c r="C4">
-        <v>30183</v>
-      </c>
-      <c r="E4" s="1">
+        <v>23366</v>
+      </c>
+      <c r="D4" s="2">
+        <v>31.560494352814601</v>
+      </c>
+      <c r="E4">
+        <v>89248</v>
+      </c>
+      <c r="F4">
+        <v>32545</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>2816710.9999999977</v>
+      </c>
+      <c r="H4">
+        <v>2816711</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>23570845</v>
+      </c>
+      <c r="B5" s="1">
         <f>(((A5)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.64166666667</v>
-      </c>
-      <c r="F4">
-        <v>23366</v>
-      </c>
-      <c r="G4" s="2">
-        <v>31.560494352814601</v>
-      </c>
-      <c r="H4">
-        <v>89248</v>
-      </c>
-      <c r="I4">
-        <v>32545</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>23570844</v>
-      </c>
-      <c r="B5">
-        <v>89248</v>
+        <v>41937.642361111109</v>
       </c>
       <c r="C5">
-        <v>32545</v>
-      </c>
-      <c r="E5" s="1">
+        <v>22102</v>
+      </c>
+      <c r="D5" s="2">
+        <v>33.350843744449001</v>
+      </c>
+      <c r="E5">
+        <v>84445</v>
+      </c>
+      <c r="F5">
+        <v>32933</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2816311.9999999958</v>
+      </c>
+      <c r="H5">
+        <v>2816312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>23570846</v>
+      </c>
+      <c r="B6" s="1">
         <f>(((A6)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.642361111109</v>
-      </c>
-      <c r="F5">
-        <v>22102</v>
-      </c>
-      <c r="G5" s="2">
-        <v>33.350843744449001</v>
-      </c>
-      <c r="H5">
-        <v>84445</v>
-      </c>
-      <c r="I5">
-        <v>32933</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>23570845</v>
-      </c>
-      <c r="B6">
-        <v>84445</v>
+        <v>41937.643055555556</v>
       </c>
       <c r="C6">
-        <v>32933</v>
-      </c>
-      <c r="E6" s="1">
+        <v>21049</v>
+      </c>
+      <c r="D6" s="2">
+        <v>35.103336948256697</v>
+      </c>
+      <c r="E6">
+        <v>80223</v>
+      </c>
+      <c r="F6">
+        <v>32814</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>2816094.9999999972</v>
+      </c>
+      <c r="H6">
+        <v>2816095</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>23570847</v>
+      </c>
+      <c r="B7" s="1">
         <f>(((A7)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.643055555556</v>
-      </c>
-      <c r="F6">
-        <v>21049</v>
-      </c>
-      <c r="G6" s="2">
-        <v>35.103336948256697</v>
-      </c>
-      <c r="H6">
-        <v>80223</v>
-      </c>
-      <c r="I6">
-        <v>32814</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>23570846</v>
-      </c>
-      <c r="B7">
-        <v>80223</v>
+        <v>41937.643750000003</v>
       </c>
       <c r="C7">
-        <v>32814</v>
-      </c>
-      <c r="E7" s="1">
+        <v>19422</v>
+      </c>
+      <c r="D7" s="2">
+        <v>38.022887989203703</v>
+      </c>
+      <c r="E7">
+        <v>74100</v>
+      </c>
+      <c r="F7">
+        <v>31620</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>2817495.9999999944</v>
+      </c>
+      <c r="H7">
+        <v>2817496</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>23570848</v>
+      </c>
+      <c r="B8" s="1">
         <f>(((A8)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.643750000003</v>
-      </c>
-      <c r="F7">
-        <v>19422</v>
-      </c>
-      <c r="G7" s="2">
-        <v>38.022887989203703</v>
-      </c>
-      <c r="H7">
-        <v>74100</v>
-      </c>
-      <c r="I7">
-        <v>31620</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>23570847</v>
-      </c>
-      <c r="B8">
-        <v>74100</v>
+        <v>41937.644444444442</v>
       </c>
       <c r="C8">
-        <v>31620</v>
-      </c>
-      <c r="E8" s="1">
+        <v>18125</v>
+      </c>
+      <c r="D8" s="2">
+        <v>40.577719497960999</v>
+      </c>
+      <c r="E8">
+        <v>69397</v>
+      </c>
+      <c r="F8">
+        <v>30257</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>2815971.9999999995</v>
+      </c>
+      <c r="H8">
+        <v>2815972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>23570849</v>
+      </c>
+      <c r="B9" s="1">
         <f>(((A9)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.644444444442</v>
-      </c>
-      <c r="F8">
-        <v>18125</v>
-      </c>
-      <c r="G8" s="2">
-        <v>40.577719497960999</v>
-      </c>
-      <c r="H8">
-        <v>69397</v>
-      </c>
-      <c r="I8">
-        <v>30257</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>23570848</v>
-      </c>
-      <c r="B9">
-        <v>69397</v>
+        <v>41937.645138888889</v>
       </c>
       <c r="C9">
-        <v>30257</v>
-      </c>
-      <c r="E9" s="1">
+        <v>16722</v>
+      </c>
+      <c r="D9" s="2">
+        <v>44.420677698975503</v>
+      </c>
+      <c r="E9">
+        <v>63450</v>
+      </c>
+      <c r="F9">
+        <v>27481</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>2818491.9999999958</v>
+      </c>
+      <c r="H9">
+        <v>2818492</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>23570850</v>
+      </c>
+      <c r="B10" s="1">
         <f>(((A10)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.645138888889</v>
-      </c>
-      <c r="F9">
-        <v>16722</v>
-      </c>
-      <c r="G9" s="2">
-        <v>44.420677698975503</v>
-      </c>
-      <c r="H9">
-        <v>63450</v>
-      </c>
-      <c r="I9">
-        <v>27481</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>23570849</v>
-      </c>
-      <c r="B10">
-        <v>63450</v>
+        <v>41937.645833333336</v>
       </c>
       <c r="C10">
-        <v>27481</v>
-      </c>
-      <c r="E10" s="1">
+        <v>14897</v>
+      </c>
+      <c r="D10" s="2">
+        <v>49.579994366593901</v>
+      </c>
+      <c r="E10">
+        <v>56804</v>
+      </c>
+      <c r="F10">
+        <v>25055</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>2816342</v>
+      </c>
+      <c r="H10">
+        <v>2816342</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>23570851</v>
+      </c>
+      <c r="B11" s="1">
         <f>(((A11)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.645833333336</v>
-      </c>
-      <c r="F10">
-        <v>14897</v>
-      </c>
-      <c r="G10" s="2">
-        <v>49.579994366593901</v>
-      </c>
-      <c r="H10">
-        <v>56804</v>
-      </c>
-      <c r="I10">
-        <v>25055</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>23570850</v>
-      </c>
-      <c r="B11">
-        <v>56804</v>
+        <v>41937.646527777775</v>
       </c>
       <c r="C11">
-        <v>25055</v>
-      </c>
-      <c r="E11" s="1">
+        <v>14461</v>
+      </c>
+      <c r="D11" s="2">
+        <v>51.189637625849599</v>
+      </c>
+      <c r="E11">
+        <v>55026</v>
+      </c>
+      <c r="F11">
+        <v>24247</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>2816761</v>
+      </c>
+      <c r="H11">
+        <v>2816761</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>23570852</v>
+      </c>
+      <c r="B12" s="1">
         <f>(((A12)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.646527777775</v>
-      </c>
-      <c r="F11">
-        <v>14461</v>
-      </c>
-      <c r="G11" s="2">
-        <v>51.189637625849599</v>
-      </c>
-      <c r="H11">
-        <v>55026</v>
-      </c>
-      <c r="I11">
-        <v>24247</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>23570851</v>
-      </c>
-      <c r="B12">
-        <v>55026</v>
+        <v>41937.647222222222</v>
       </c>
       <c r="C12">
-        <v>24247</v>
-      </c>
-      <c r="E12" s="1">
+        <v>14214</v>
+      </c>
+      <c r="D12" s="2">
+        <v>52.065780964171502</v>
+      </c>
+      <c r="E12">
+        <v>54119</v>
+      </c>
+      <c r="F12">
+        <v>23873</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2817747.9999999977</v>
+      </c>
+      <c r="H12">
+        <v>2817748</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>23570853</v>
+      </c>
+      <c r="B13" s="1">
         <f>(((A13)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.647222222222</v>
-      </c>
-      <c r="F12">
-        <v>14214</v>
-      </c>
-      <c r="G12" s="2">
-        <v>52.065780964171502</v>
-      </c>
-      <c r="H12">
-        <v>54119</v>
-      </c>
-      <c r="I12">
-        <v>23873</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>23570852</v>
-      </c>
-      <c r="B13">
-        <v>54119</v>
+        <v>41937.647916666669</v>
       </c>
       <c r="C13">
-        <v>23873</v>
-      </c>
-      <c r="E13" s="1">
+        <v>13707</v>
+      </c>
+      <c r="D13" s="2">
+        <v>53.983121635342997</v>
+      </c>
+      <c r="E13">
+        <v>52197</v>
+      </c>
+      <c r="F13">
+        <v>23346</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>2817756.9999999986</v>
+      </c>
+      <c r="H13">
+        <v>2817757</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>23570854</v>
+      </c>
+      <c r="B14" s="1">
         <f>(((A14)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.647916666669</v>
-      </c>
-      <c r="F13">
-        <v>13707</v>
-      </c>
-      <c r="G13" s="2">
-        <v>53.983121635342997</v>
-      </c>
-      <c r="H13">
-        <v>52197</v>
-      </c>
-      <c r="I13">
-        <v>23346</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>23570853</v>
-      </c>
-      <c r="B14">
-        <v>52197</v>
+        <v>41937.648611111108</v>
       </c>
       <c r="C14">
-        <v>23346</v>
-      </c>
-      <c r="E14" s="1">
+        <v>13431</v>
+      </c>
+      <c r="D14" s="2">
+        <v>55.412793897931898</v>
+      </c>
+      <c r="E14">
+        <v>50868</v>
+      </c>
+      <c r="F14">
+        <v>22616</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>2818738</v>
+      </c>
+      <c r="H14">
+        <v>2818738</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>23570855</v>
+      </c>
+      <c r="B15" s="1">
         <f>(((A15)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.648611111108</v>
-      </c>
-      <c r="F14">
-        <v>13431</v>
-      </c>
-      <c r="G14" s="2">
-        <v>55.412793897931898</v>
-      </c>
-      <c r="H14">
-        <v>50868</v>
-      </c>
-      <c r="I14">
-        <v>22616</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>23570854</v>
-      </c>
-      <c r="B15">
-        <v>50868</v>
+        <v>41937.649305555555</v>
       </c>
       <c r="C15">
-        <v>22616</v>
-      </c>
-      <c r="E15" s="1">
+        <v>13228</v>
+      </c>
+      <c r="D15" s="2">
+        <v>56.267816114918098</v>
+      </c>
+      <c r="E15">
+        <v>50053</v>
+      </c>
+      <c r="F15">
+        <v>22196</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>2816372.9999999953</v>
+      </c>
+      <c r="H15">
+        <v>2816373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>23570856</v>
+      </c>
+      <c r="B16" s="1">
         <f>(((A16)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.649305555555</v>
-      </c>
-      <c r="F15">
-        <v>13228</v>
-      </c>
-      <c r="G15" s="2">
-        <v>56.267816114918098</v>
-      </c>
-      <c r="H15">
-        <v>50053</v>
-      </c>
-      <c r="I15">
-        <v>22196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>23570855</v>
-      </c>
-      <c r="B16">
-        <v>50053</v>
+        <v>41937.65</v>
       </c>
       <c r="C16">
-        <v>22196</v>
-      </c>
-      <c r="E16" s="1">
+        <v>12647</v>
+      </c>
+      <c r="D16" s="2">
+        <v>59.185815066767397</v>
+      </c>
+      <c r="E16">
+        <v>47628</v>
+      </c>
+      <c r="F16">
+        <v>21171</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>2818901.9999999977</v>
+      </c>
+      <c r="H16">
+        <v>2818902</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>23570857</v>
+      </c>
+      <c r="B17" s="1">
         <f>(((A17)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.65</v>
-      </c>
-      <c r="F16">
-        <v>12647</v>
-      </c>
-      <c r="G16" s="2">
-        <v>59.185815066767397</v>
-      </c>
-      <c r="H16">
-        <v>47628</v>
-      </c>
-      <c r="I16">
-        <v>21171</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>23570856</v>
-      </c>
-      <c r="B17">
-        <v>47628</v>
+        <v>41937.650694444441</v>
       </c>
       <c r="C17">
-        <v>21171</v>
-      </c>
-      <c r="E17" s="1">
+        <v>12479</v>
+      </c>
+      <c r="D17" s="2">
+        <v>60.022043618223201</v>
+      </c>
+      <c r="E17">
+        <v>46907</v>
+      </c>
+      <c r="F17">
+        <v>20731</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>2815453.9999999958</v>
+      </c>
+      <c r="H17">
+        <v>2815454</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>23570858</v>
+      </c>
+      <c r="B18" s="1">
         <f>(((A18)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.650694444441</v>
-      </c>
-      <c r="F17">
-        <v>12479</v>
-      </c>
-      <c r="G17" s="2">
-        <v>60.022043618223201</v>
-      </c>
-      <c r="H17">
-        <v>46907</v>
-      </c>
-      <c r="I17">
-        <v>20731</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>23570857</v>
-      </c>
-      <c r="B18">
-        <v>46907</v>
+        <v>41937.651388888888</v>
       </c>
       <c r="C18">
-        <v>20731</v>
-      </c>
-      <c r="E18" s="1">
+        <v>12028</v>
+      </c>
+      <c r="D18" s="2">
+        <v>62.395655735889903</v>
+      </c>
+      <c r="E18">
+        <v>45163</v>
+      </c>
+      <c r="F18">
+        <v>20153</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>2817974.9999999958</v>
+      </c>
+      <c r="H18">
+        <v>2817975</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>23570859</v>
+      </c>
+      <c r="B19" s="1">
         <f>(((A19)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.651388888888</v>
-      </c>
-      <c r="F18">
-        <v>12028</v>
-      </c>
-      <c r="G18" s="2">
-        <v>62.395655735889903</v>
-      </c>
-      <c r="H18">
-        <v>45163</v>
-      </c>
-      <c r="I18">
-        <v>20153</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>23570858</v>
-      </c>
-      <c r="B19">
-        <v>45163</v>
+        <v>41937.652083333334</v>
       </c>
       <c r="C19">
-        <v>20153</v>
-      </c>
-      <c r="E19" s="1">
+        <v>12043</v>
+      </c>
+      <c r="D19" s="2">
+        <v>62.214995363624297</v>
+      </c>
+      <c r="E19">
+        <v>45294</v>
+      </c>
+      <c r="F19">
+        <v>20267</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>2817965.9999999991</v>
+      </c>
+      <c r="H19">
+        <v>2817966</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>23570860</v>
+      </c>
+      <c r="B20" s="1">
         <f>(((A20)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.652083333334</v>
-      </c>
-      <c r="F19">
-        <v>12043</v>
-      </c>
-      <c r="G19" s="2">
-        <v>62.214995363624297</v>
-      </c>
-      <c r="H19">
-        <v>45294</v>
-      </c>
-      <c r="I19">
-        <v>20267</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>23570859</v>
-      </c>
-      <c r="B20">
-        <v>45294</v>
+        <v>41937.652777777781</v>
       </c>
       <c r="C20">
-        <v>20267</v>
-      </c>
-      <c r="E20" s="1">
+        <v>11723</v>
+      </c>
+      <c r="D20" s="2">
+        <v>63.424607553883902</v>
+      </c>
+      <c r="E20">
+        <v>44401</v>
+      </c>
+      <c r="F20">
+        <v>19842</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>2816115.9999999991</v>
+      </c>
+      <c r="H20">
+        <v>2816116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>23570861</v>
+      </c>
+      <c r="B21" s="1">
         <f>(((A21)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.652777777781</v>
-      </c>
-      <c r="F20">
-        <v>11723</v>
-      </c>
-      <c r="G20" s="2">
-        <v>63.424607553883902</v>
-      </c>
-      <c r="H20">
-        <v>44401</v>
-      </c>
-      <c r="I20">
-        <v>19842</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>23570860</v>
-      </c>
-      <c r="B21">
-        <v>44401</v>
+        <v>41937.65347222222</v>
       </c>
       <c r="C21">
-        <v>19842</v>
-      </c>
-      <c r="E21" s="1">
+        <v>11232</v>
+      </c>
+      <c r="D21" s="2">
+        <v>66.064495709663802</v>
+      </c>
+      <c r="E21">
+        <v>42654</v>
+      </c>
+      <c r="F21">
+        <v>18841</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>2817915</v>
+      </c>
+      <c r="H21">
+        <v>2817915</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>23570862</v>
+      </c>
+      <c r="B22" s="1">
         <f>(((A22)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.65347222222</v>
-      </c>
-      <c r="F21">
-        <v>11232</v>
-      </c>
-      <c r="G21" s="2">
-        <v>66.064495709663802</v>
-      </c>
-      <c r="H21">
-        <v>42654</v>
-      </c>
-      <c r="I21">
-        <v>18841</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>23570861</v>
-      </c>
-      <c r="B22">
-        <v>42654</v>
+        <v>41937.654166666667</v>
       </c>
       <c r="C22">
-        <v>18841</v>
-      </c>
-      <c r="E22" s="1">
+        <v>11341</v>
+      </c>
+      <c r="D22" s="2">
+        <v>65.271383217852701</v>
+      </c>
+      <c r="E22">
+        <v>43153</v>
+      </c>
+      <c r="F22">
+        <v>18990</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>2816655.9999999977</v>
+      </c>
+      <c r="H22">
+        <v>2816656</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>23570863</v>
+      </c>
+      <c r="B23" s="1">
         <f>(((A23)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.654166666667</v>
-      </c>
-      <c r="F22">
-        <v>11341</v>
-      </c>
-      <c r="G22" s="2">
-        <v>65.271383217852701</v>
-      </c>
-      <c r="H22">
-        <v>43153</v>
-      </c>
-      <c r="I22">
-        <v>18990</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>23570862</v>
-      </c>
-      <c r="B23">
-        <v>43153</v>
+        <v>41937.654861111114</v>
       </c>
       <c r="C23">
-        <v>18990</v>
-      </c>
-      <c r="E23" s="1">
+        <v>11029</v>
+      </c>
+      <c r="D23" s="2">
+        <v>67.253996659508402</v>
+      </c>
+      <c r="E23">
+        <v>41910</v>
+      </c>
+      <c r="F23">
+        <v>18519</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>2818614.9999999972</v>
+      </c>
+      <c r="H23">
+        <v>2818615</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23570864</v>
+      </c>
+      <c r="B24" s="1">
         <f>(((A24)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.654861111114</v>
-      </c>
-      <c r="F23">
-        <v>11029</v>
-      </c>
-      <c r="G23" s="2">
-        <v>67.253996659508402</v>
-      </c>
-      <c r="H23">
-        <v>41910</v>
-      </c>
-      <c r="I23">
-        <v>18519</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>23570863</v>
-      </c>
-      <c r="B24">
-        <v>41910</v>
+        <v>41937.655555555553</v>
       </c>
       <c r="C24">
-        <v>18519</v>
-      </c>
-      <c r="E24" s="1">
+        <v>11030</v>
+      </c>
+      <c r="D24" s="2">
+        <v>67.301913841301698</v>
+      </c>
+      <c r="E24">
+        <v>41853</v>
+      </c>
+      <c r="F24">
+        <v>18297</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>2816787</v>
+      </c>
+      <c r="H24">
+        <v>2816787</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23570865</v>
+      </c>
+      <c r="B25" s="1">
         <f>(((A25)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.655555555553</v>
-      </c>
-      <c r="F24">
-        <v>11030</v>
-      </c>
-      <c r="G24" s="2">
-        <v>67.301913841301698</v>
-      </c>
-      <c r="H24">
-        <v>41853</v>
-      </c>
-      <c r="I24">
-        <v>18297</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>23570864</v>
-      </c>
-      <c r="B25">
-        <v>41853</v>
+        <v>41937.65625</v>
       </c>
       <c r="C25">
-        <v>18297</v>
-      </c>
-      <c r="E25" s="1">
+        <v>10764</v>
+      </c>
+      <c r="D25" s="2">
+        <v>68.947488193407807</v>
+      </c>
+      <c r="E25">
+        <v>40867</v>
+      </c>
+      <c r="F25">
+        <v>17905</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>2817676.9999999967</v>
+      </c>
+      <c r="H25">
+        <v>2817677</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>23570866</v>
+      </c>
+      <c r="B26" s="1">
         <f>(((A26)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.65625</v>
-      </c>
-      <c r="F25">
-        <v>10764</v>
-      </c>
-      <c r="G25" s="2">
-        <v>68.947488193407807</v>
-      </c>
-      <c r="H25">
-        <v>40867</v>
-      </c>
-      <c r="I25">
-        <v>17905</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>23570865</v>
-      </c>
-      <c r="B26">
-        <v>40867</v>
+        <v>41937.656944444447</v>
       </c>
       <c r="C26">
-        <v>17905</v>
-      </c>
-      <c r="E26" s="1">
+        <v>10815</v>
+      </c>
+      <c r="D26" s="2">
+        <v>69.278909556146004</v>
+      </c>
+      <c r="E26">
+        <v>40644</v>
+      </c>
+      <c r="F26">
+        <v>17851</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>2815771.9999999981</v>
+      </c>
+      <c r="H26">
+        <v>2815772</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>23570867</v>
+      </c>
+      <c r="B27" s="1">
         <f>(((A27)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.656944444447</v>
-      </c>
-      <c r="F26">
-        <v>10815</v>
-      </c>
-      <c r="G26" s="2">
-        <v>69.278909556146004</v>
-      </c>
-      <c r="H26">
-        <v>40644</v>
-      </c>
-      <c r="I26">
-        <v>17851</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>23570866</v>
-      </c>
-      <c r="B27">
-        <v>40644</v>
+        <v>41937.657638888886</v>
       </c>
       <c r="C27">
-        <v>17851</v>
-      </c>
-      <c r="E27" s="1">
+        <v>10390</v>
+      </c>
+      <c r="D27" s="2">
+        <v>71.233959212554595</v>
+      </c>
+      <c r="E27">
+        <v>39571</v>
+      </c>
+      <c r="F27">
+        <v>17418</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>2818798.9999999977</v>
+      </c>
+      <c r="H27">
+        <v>2818799</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>23570868</v>
+      </c>
+      <c r="B28" s="1">
         <f>(((A28)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.657638888886</v>
-      </c>
-      <c r="F27">
-        <v>10390</v>
-      </c>
-      <c r="G27" s="2">
-        <v>71.233959212554595</v>
-      </c>
-      <c r="H27">
-        <v>39571</v>
-      </c>
-      <c r="I27">
-        <v>17418</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>23570867</v>
-      </c>
-      <c r="B28">
-        <v>39571</v>
+        <v>41937.658333333333</v>
       </c>
       <c r="C28">
-        <v>17418</v>
-      </c>
-      <c r="E28" s="1">
+        <v>10292</v>
+      </c>
+      <c r="D28" s="2">
+        <v>72.083823905809993</v>
+      </c>
+      <c r="E28">
+        <v>39070</v>
+      </c>
+      <c r="F28">
+        <v>16993</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>2816314.9999999963</v>
+      </c>
+      <c r="H28">
+        <v>2816315</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>23570869</v>
+      </c>
+      <c r="B29" s="1">
         <f>(((A29)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.658333333333</v>
-      </c>
-      <c r="F28">
-        <v>10292</v>
-      </c>
-      <c r="G28" s="2">
-        <v>72.083823905809993</v>
-      </c>
-      <c r="H28">
-        <v>39070</v>
-      </c>
-      <c r="I28">
-        <v>16993</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>23570868</v>
-      </c>
-      <c r="B29">
-        <v>39070</v>
+        <v>41937.65902777778</v>
       </c>
       <c r="C29">
-        <v>16993</v>
-      </c>
-      <c r="E29" s="1">
+        <v>10189</v>
+      </c>
+      <c r="D29" s="2">
+        <v>73.450701287866906</v>
+      </c>
+      <c r="E29">
+        <v>38358</v>
+      </c>
+      <c r="F29">
+        <v>16635</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>2817421.9999999986</v>
+      </c>
+      <c r="H29">
+        <v>2817422</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>23570870</v>
+      </c>
+      <c r="B30" s="1">
         <f>(((A30)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.65902777778</v>
-      </c>
-      <c r="F29">
-        <v>10189</v>
-      </c>
-      <c r="G29" s="2">
-        <v>73.450701287866906</v>
-      </c>
-      <c r="H29">
-        <v>38358</v>
-      </c>
-      <c r="I29">
-        <v>16635</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>23570869</v>
-      </c>
-      <c r="B30">
-        <v>38358</v>
+        <v>41937.659722222219</v>
       </c>
       <c r="C30">
-        <v>16635</v>
-      </c>
-      <c r="E30" s="1">
+        <v>9877</v>
+      </c>
+      <c r="D30" s="2">
+        <v>75.017625602385493</v>
+      </c>
+      <c r="E30">
+        <v>37559</v>
+      </c>
+      <c r="F30">
+        <v>16288</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>2817586.9999999967</v>
+      </c>
+      <c r="H30">
+        <v>2817587</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>23570871</v>
+      </c>
+      <c r="B31" s="1">
         <f>(((A31)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.659722222219</v>
-      </c>
-      <c r="F30">
-        <v>9877</v>
-      </c>
-      <c r="G30" s="2">
-        <v>75.017625602385493</v>
-      </c>
-      <c r="H30">
-        <v>37559</v>
-      </c>
-      <c r="I30">
-        <v>16288</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>23570870</v>
-      </c>
-      <c r="B31">
-        <v>37559</v>
+        <v>41937.660416666666</v>
       </c>
       <c r="C31">
-        <v>16288</v>
-      </c>
-      <c r="E31" s="1">
+        <v>10010</v>
+      </c>
+      <c r="D31" s="2">
+        <v>74.884299715795905</v>
+      </c>
+      <c r="E31">
+        <v>37649</v>
+      </c>
+      <c r="F31">
+        <v>16335</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>2819319</v>
+      </c>
+      <c r="H31">
+        <v>2819319</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>23570872</v>
+      </c>
+      <c r="B32" s="1">
         <f>(((A32)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.660416666666</v>
-      </c>
-      <c r="F31">
-        <v>10010</v>
-      </c>
-      <c r="G31" s="2">
-        <v>74.884299715795905</v>
-      </c>
-      <c r="H31">
-        <v>37649</v>
-      </c>
-      <c r="I31">
-        <v>16335</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>23570871</v>
-      </c>
-      <c r="B32">
-        <v>37649</v>
+        <v>41937.661111111112</v>
       </c>
       <c r="C32">
-        <v>16335</v>
-      </c>
-      <c r="E32" s="1">
+        <v>9805</v>
+      </c>
+      <c r="D32" s="2">
+        <v>75.3307394036635</v>
+      </c>
+      <c r="E32">
+        <v>37395</v>
+      </c>
+      <c r="F32">
+        <v>16061</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>2816992.9999999967</v>
+      </c>
+      <c r="H32">
+        <v>2816993</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>23570873</v>
+      </c>
+      <c r="B33" s="1">
         <f>(((A33)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.661111111112</v>
-      </c>
-      <c r="F32">
-        <v>9805</v>
-      </c>
-      <c r="G32" s="2">
-        <v>75.3307394036635</v>
-      </c>
-      <c r="H32">
-        <v>37395</v>
-      </c>
-      <c r="I32">
-        <v>16061</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>23570872</v>
-      </c>
-      <c r="B33">
-        <v>37395</v>
+        <v>41937.661805555559</v>
       </c>
       <c r="C33">
-        <v>16061</v>
-      </c>
-      <c r="E33" s="1">
+        <v>9768</v>
+      </c>
+      <c r="D33" s="2">
+        <v>76.205096299502202</v>
+      </c>
+      <c r="E33">
+        <v>36968</v>
+      </c>
+      <c r="F33">
+        <v>15884</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>2817149.9999999972</v>
+      </c>
+      <c r="H33">
+        <v>2817150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>23570874</v>
+      </c>
+      <c r="B34" s="1">
         <f>(((A34)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.661805555559</v>
-      </c>
-      <c r="F33">
-        <v>9768</v>
-      </c>
-      <c r="G33" s="2">
-        <v>76.205096299502202</v>
-      </c>
-      <c r="H33">
-        <v>36968</v>
-      </c>
-      <c r="I33">
-        <v>15884</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>23570873</v>
-      </c>
-      <c r="B34">
-        <v>36968</v>
+        <v>41937.662499999999</v>
       </c>
       <c r="C34">
-        <v>15884</v>
-      </c>
-      <c r="E34" s="1">
+        <v>9556</v>
+      </c>
+      <c r="D34" s="2">
+        <v>78.113880878438295</v>
+      </c>
+      <c r="E34">
+        <v>36064</v>
+      </c>
+      <c r="F34">
+        <v>15748</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>2817098.9999999986</v>
+      </c>
+      <c r="H34">
+        <v>2817099</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>23570875</v>
+      </c>
+      <c r="B35" s="1">
         <f>(((A35)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.662499999999</v>
-      </c>
-      <c r="F34">
-        <v>9556</v>
-      </c>
-      <c r="G34" s="2">
-        <v>78.113880878438295</v>
-      </c>
-      <c r="H34">
-        <v>36064</v>
-      </c>
-      <c r="I34">
-        <v>15748</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>23570874</v>
-      </c>
-      <c r="B35">
-        <v>36064</v>
+        <v>41937.663194444445</v>
       </c>
       <c r="C35">
-        <v>15748</v>
-      </c>
-      <c r="E35" s="1">
+        <v>8995</v>
+      </c>
+      <c r="D35" s="2">
+        <v>82.531505165500803</v>
+      </c>
+      <c r="E35">
+        <v>34169</v>
+      </c>
+      <c r="F35">
+        <v>14650</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>2820018.9999999967</v>
+      </c>
+      <c r="H35">
+        <v>2820019</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>23570876</v>
+      </c>
+      <c r="B36" s="1">
         <f>(((A36)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.663194444445</v>
-      </c>
-      <c r="F35">
+        <v>41937.663888888892</v>
+      </c>
+      <c r="C36">
+        <v>9002</v>
+      </c>
+      <c r="D36" s="2">
+        <v>82.278410750803303</v>
+      </c>
+      <c r="E36">
+        <v>34230</v>
+      </c>
+      <c r="F36">
+        <v>14631</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>2816389.9999999972</v>
+      </c>
+      <c r="H36">
+        <v>2816390</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>23570877</v>
+      </c>
+      <c r="B37" s="1">
+        <f>(((A37)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.664583333331</v>
+      </c>
+      <c r="C37">
+        <v>9151</v>
+      </c>
+      <c r="D37" s="2">
+        <v>81.690236763555205</v>
+      </c>
+      <c r="E37">
+        <v>34507</v>
+      </c>
+      <c r="F37">
+        <v>14749</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>2818884.9999999995</v>
+      </c>
+      <c r="H37">
+        <v>2818885</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>23570878</v>
+      </c>
+      <c r="B38" s="1">
+        <f>(((A38)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.665277777778</v>
+      </c>
+      <c r="C38">
         <v>8995</v>
       </c>
-      <c r="G35" s="2">
-        <v>82.531505165500803</v>
-      </c>
-      <c r="H35">
-        <v>34169</v>
-      </c>
-      <c r="I35">
-        <v>14650</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>23570875</v>
-      </c>
-      <c r="B36">
-        <v>34169</v>
-      </c>
-      <c r="C36">
-        <v>14650</v>
-      </c>
-      <c r="E36" s="1">
-        <f>(((A37)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.663888888892</v>
-      </c>
-      <c r="F36">
-        <v>9002</v>
-      </c>
-      <c r="G36" s="2">
-        <v>82.278410750803303</v>
-      </c>
-      <c r="H36">
-        <v>34230</v>
-      </c>
-      <c r="I36">
-        <v>14631</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>23570876</v>
-      </c>
-      <c r="B37">
-        <v>34230</v>
-      </c>
-      <c r="C37">
-        <v>14631</v>
-      </c>
-      <c r="E37" s="1">
-        <f>(((A38)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.664583333331</v>
-      </c>
-      <c r="F37">
-        <v>9151</v>
-      </c>
-      <c r="G37" s="2">
-        <v>81.690236763555205</v>
-      </c>
-      <c r="H37">
-        <v>34507</v>
-      </c>
-      <c r="I37">
-        <v>14749</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>23570877</v>
-      </c>
-      <c r="B38">
-        <v>34507</v>
-      </c>
-      <c r="C38">
-        <v>14749</v>
-      </c>
-      <c r="E38" s="1">
+      <c r="D38" s="2">
+        <v>82.642553191489299</v>
+      </c>
+      <c r="E38">
+        <v>34075</v>
+      </c>
+      <c r="F38">
+        <v>14486</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>2816044.9999999977</v>
+      </c>
+      <c r="H38">
+        <v>2816045</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>23570879</v>
+      </c>
+      <c r="B39" s="1">
         <f>(((A39)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.665277777778</v>
-      </c>
-      <c r="F38">
-        <v>8995</v>
-      </c>
-      <c r="G38" s="2">
-        <v>82.642553191489299</v>
-      </c>
-      <c r="H38">
-        <v>34075</v>
-      </c>
-      <c r="I38">
-        <v>14486</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>23570878</v>
-      </c>
-      <c r="B39">
-        <v>34075</v>
+        <v>41937.665972222225</v>
       </c>
       <c r="C39">
-        <v>14486</v>
-      </c>
-      <c r="E39" s="1">
+        <v>9032</v>
+      </c>
+      <c r="D39" s="2">
+        <v>81.772075887676905</v>
+      </c>
+      <c r="E39">
+        <v>34472</v>
+      </c>
+      <c r="F39">
+        <v>14899</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>2818846.9999999981</v>
+      </c>
+      <c r="H39">
+        <v>2818847</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>23570880</v>
+      </c>
+      <c r="B40" s="1">
         <f>(((A40)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.665972222225</v>
-      </c>
-      <c r="F39">
-        <v>9032</v>
-      </c>
-      <c r="G39" s="2">
-        <v>81.772075887676905</v>
-      </c>
-      <c r="H39">
-        <v>34472</v>
-      </c>
-      <c r="I39">
-        <v>14899</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>23570879</v>
-      </c>
-      <c r="B40">
-        <v>34472</v>
+        <v>41937.666666666664</v>
       </c>
       <c r="C40">
-        <v>14899</v>
-      </c>
-      <c r="E40" s="1">
+        <v>8819</v>
+      </c>
+      <c r="D40" s="2">
+        <v>84.482169101106706</v>
+      </c>
+      <c r="E40">
+        <v>33341</v>
+      </c>
+      <c r="F40">
+        <v>14088</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>2816719.9999999986</v>
+      </c>
+      <c r="H40">
+        <v>2816720</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>23570881</v>
+      </c>
+      <c r="B41" s="1">
         <f>(((A41)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.666666666664</v>
-      </c>
-      <c r="F40">
-        <v>8819</v>
-      </c>
-      <c r="G40" s="2">
-        <v>84.482169101106706</v>
-      </c>
-      <c r="H40">
-        <v>33341</v>
-      </c>
-      <c r="I40">
-        <v>14088</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>23570880</v>
-      </c>
-      <c r="B41">
-        <v>33341</v>
+        <v>41937.667361111111</v>
       </c>
       <c r="C41">
-        <v>14088</v>
-      </c>
-      <c r="E41" s="1">
+        <v>8755</v>
+      </c>
+      <c r="D41" s="2">
+        <v>84.006794207044507</v>
+      </c>
+      <c r="E41">
+        <v>33558</v>
+      </c>
+      <c r="F41">
+        <v>14120</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>2819099.9999999995</v>
+      </c>
+      <c r="H41">
+        <v>2819100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>23570882</v>
+      </c>
+      <c r="B42" s="1">
         <f>(((A42)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.667361111111</v>
-      </c>
-      <c r="F41">
-        <v>8755</v>
-      </c>
-      <c r="G41" s="2">
-        <v>84.006794207044507</v>
-      </c>
-      <c r="H41">
-        <v>33558</v>
-      </c>
-      <c r="I41">
-        <v>14120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>23570881</v>
-      </c>
-      <c r="B42">
-        <v>33558</v>
+        <v>41937.668055555558</v>
       </c>
       <c r="C42">
-        <v>14120</v>
-      </c>
-      <c r="E42" s="1">
+        <v>8707</v>
+      </c>
+      <c r="D42" s="2">
+        <v>84.517107869620006</v>
+      </c>
+      <c r="E42">
+        <v>33318</v>
+      </c>
+      <c r="F42">
+        <v>14225</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>2815940.9999999995</v>
+      </c>
+      <c r="H42">
+        <v>2815941</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>23570883</v>
+      </c>
+      <c r="B43" s="1">
         <f>(((A43)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.668055555558</v>
-      </c>
-      <c r="F42">
-        <v>8707</v>
-      </c>
-      <c r="G42" s="2">
-        <v>84.517107869620006</v>
-      </c>
-      <c r="H42">
-        <v>33318</v>
-      </c>
-      <c r="I42">
-        <v>14225</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>23570882</v>
-      </c>
-      <c r="B43">
-        <v>33318</v>
+        <v>41937.668749999997</v>
       </c>
       <c r="C43">
-        <v>14225</v>
-      </c>
-      <c r="E43" s="1">
+        <v>8687</v>
+      </c>
+      <c r="D43" s="2">
+        <v>85.642924399356005</v>
+      </c>
+      <c r="E43">
+        <v>32923</v>
+      </c>
+      <c r="F43">
+        <v>14068</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>2819621.9999999977</v>
+      </c>
+      <c r="H43">
+        <v>2819622</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>23570884</v>
+      </c>
+      <c r="B44" s="1">
         <f>(((A44)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.668749999997</v>
-      </c>
-      <c r="F43">
-        <v>8687</v>
-      </c>
-      <c r="G43" s="2">
-        <v>85.642924399356005</v>
-      </c>
-      <c r="H43">
-        <v>32923</v>
-      </c>
-      <c r="I43">
-        <v>14068</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>23570883</v>
-      </c>
-      <c r="B44">
-        <v>32923</v>
+        <v>41937.669444444444</v>
       </c>
       <c r="C44">
-        <v>14068</v>
-      </c>
-      <c r="E44" s="1">
+        <v>8458</v>
+      </c>
+      <c r="D44" s="2">
+        <v>87.626929780876495</v>
+      </c>
+      <c r="E44">
+        <v>32128</v>
+      </c>
+      <c r="F44">
+        <v>13558</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>2815278</v>
+      </c>
+      <c r="H44">
+        <v>2815278</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>23570885</v>
+      </c>
+      <c r="B45" s="1">
         <f>(((A45)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.669444444444</v>
-      </c>
-      <c r="F44">
-        <v>8458</v>
-      </c>
-      <c r="G44" s="2">
-        <v>87.626929780876495</v>
-      </c>
-      <c r="H44">
-        <v>32128</v>
-      </c>
-      <c r="I44">
-        <v>13558</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>23570884</v>
-      </c>
-      <c r="B45">
-        <v>32128</v>
+        <v>41937.670138888891</v>
       </c>
       <c r="C45">
-        <v>13558</v>
-      </c>
-      <c r="E45" s="1">
+        <v>8463</v>
+      </c>
+      <c r="D45" s="2">
+        <v>88.971570852244</v>
+      </c>
+      <c r="E45">
+        <v>31728</v>
+      </c>
+      <c r="F45">
+        <v>13324</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>2822889.9999999977</v>
+      </c>
+      <c r="H45">
+        <v>2822890</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>23570886</v>
+      </c>
+      <c r="B46" s="1">
         <f>(((A46)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.670138888891</v>
-      </c>
-      <c r="F45">
-        <v>8463</v>
-      </c>
-      <c r="G45" s="2">
-        <v>88.971570852244</v>
-      </c>
-      <c r="H45">
-        <v>31728</v>
-      </c>
-      <c r="I45">
-        <v>13324</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>23570885</v>
-      </c>
-      <c r="B46">
-        <v>31728</v>
+        <v>41937.67083333333</v>
       </c>
       <c r="C46">
-        <v>13324</v>
-      </c>
-      <c r="E46" s="1">
+        <v>8218</v>
+      </c>
+      <c r="D46" s="2">
+        <v>90.647721783931701</v>
+      </c>
+      <c r="E46">
+        <v>31055</v>
+      </c>
+      <c r="F46">
+        <v>13042</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>2815064.9999999991</v>
+      </c>
+      <c r="H46">
+        <v>2815065</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>23570887</v>
+      </c>
+      <c r="B47" s="1">
         <f>(((A47)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.67083333333</v>
-      </c>
-      <c r="F46">
-        <v>8218</v>
-      </c>
-      <c r="G46" s="2">
-        <v>90.647721783931701</v>
-      </c>
-      <c r="H46">
-        <v>31055</v>
-      </c>
-      <c r="I46">
-        <v>13042</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>23570886</v>
-      </c>
-      <c r="B47">
-        <v>31055</v>
+        <v>41937.671527777777</v>
       </c>
       <c r="C47">
-        <v>13042</v>
-      </c>
-      <c r="E47" s="1">
+        <v>8374</v>
+      </c>
+      <c r="D47" s="2">
+        <v>89.903793994702994</v>
+      </c>
+      <c r="E47">
+        <v>31339</v>
+      </c>
+      <c r="F47">
+        <v>13004</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>2817494.9999999972</v>
+      </c>
+      <c r="H47">
+        <v>2817495</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>23570888</v>
+      </c>
+      <c r="B48" s="1">
         <f>(((A48)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.671527777777</v>
-      </c>
-      <c r="F47">
-        <v>8374</v>
-      </c>
-      <c r="G47" s="2">
-        <v>89.903793994702994</v>
-      </c>
-      <c r="H47">
-        <v>31339</v>
-      </c>
-      <c r="I47">
-        <v>13004</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>23570887</v>
-      </c>
-      <c r="B48">
-        <v>31339</v>
+        <v>41937.672222222223</v>
       </c>
       <c r="C48">
-        <v>13004</v>
-      </c>
-      <c r="E48" s="1">
-        <f>(((A49)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.672222222223</v>
+        <v>8261</v>
+      </c>
+      <c r="D48" s="2">
+        <v>90.415836190598199</v>
+      </c>
+      <c r="E48">
+        <v>31207</v>
       </c>
       <c r="F48">
-        <v>8261</v>
-      </c>
-      <c r="G48" s="2">
-        <v>90.415836190598199</v>
+        <v>12951</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>2821606.9999999981</v>
       </c>
       <c r="H48">
-        <v>31207</v>
-      </c>
-      <c r="I48">
-        <v>12951</v>
+        <v>2821607</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>23570888</v>
-      </c>
-      <c r="B49">
-        <v>31207</v>
+        <v>23570889</v>
+      </c>
+      <c r="B49" s="1">
+        <f>(((A49)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.67291666667</v>
       </c>
       <c r="C49">
-        <v>12951</v>
-      </c>
-      <c r="E49" s="1">
-        <f>(((A50)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.67291666667</v>
+        <v>8096</v>
+      </c>
+      <c r="D49" s="2">
+        <v>89.568963836631198</v>
+      </c>
+      <c r="E49">
+        <v>30777</v>
       </c>
       <c r="F49">
-        <v>8096</v>
-      </c>
-      <c r="G49" s="2">
-        <v>89.568963836631198</v>
+        <v>12941</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>2756663.9999999986</v>
       </c>
       <c r="H49">
-        <v>30777</v>
-      </c>
-      <c r="I49">
-        <v>12941</v>
+        <v>2756664</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>23570889</v>
-      </c>
-      <c r="B50">
-        <v>30777</v>
+        <v>23570890</v>
+      </c>
+      <c r="B50" s="1">
+        <f>(((A50)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.673611111109</v>
       </c>
       <c r="C50">
-        <v>12941</v>
-      </c>
-      <c r="E50" s="1">
-        <f>(((A51)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.673611111109</v>
+        <v>11708</v>
+      </c>
+      <c r="D50" s="2">
+        <v>61.676630341953299</v>
+      </c>
+      <c r="E50">
+        <v>29273</v>
       </c>
       <c r="F50">
-        <v>11708</v>
-      </c>
-      <c r="G50" s="2">
-        <v>61.676630341953299</v>
+        <v>12187</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>1805459.9999999988</v>
       </c>
       <c r="H50">
-        <v>29273</v>
-      </c>
-      <c r="I50">
-        <v>12187</v>
+        <v>1805460</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>23570890</v>
-      </c>
-      <c r="B51">
-        <v>29273</v>
+        <v>23570891</v>
+      </c>
+      <c r="B51" s="1">
+        <f>(((A51)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.674305555556</v>
       </c>
       <c r="C51">
-        <v>12187</v>
-      </c>
-      <c r="E51" s="1">
-        <f>(((A52)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.674305555556</v>
+        <v>14966</v>
+      </c>
+      <c r="D51" s="2">
+        <v>51.428112048020502</v>
+      </c>
+      <c r="E51">
+        <v>27988</v>
       </c>
       <c r="F51">
-        <v>14966</v>
-      </c>
-      <c r="G51" s="2">
-        <v>51.428112048020502</v>
+        <v>11418</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>1439369.9999999979</v>
       </c>
       <c r="H51">
-        <v>27988</v>
-      </c>
-      <c r="I51">
-        <v>11418</v>
+        <v>1439370</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>23570891</v>
-      </c>
-      <c r="B52">
-        <v>27988</v>
+        <v>23570892</v>
+      </c>
+      <c r="B52" s="1">
+        <f>(((A52)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.675000000003</v>
       </c>
       <c r="C52">
-        <v>11418</v>
-      </c>
-      <c r="E52" s="1">
-        <f>(((A53)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.675000000003</v>
+        <v>15136</v>
+      </c>
+      <c r="D52" s="2">
+        <v>50.955232888383897</v>
+      </c>
+      <c r="E52">
+        <v>28168</v>
       </c>
       <c r="F52">
-        <v>15136</v>
-      </c>
-      <c r="G52" s="2">
-        <v>50.955232888383897</v>
+        <v>11706</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>1435306.9999999977</v>
       </c>
       <c r="H52">
-        <v>28168</v>
-      </c>
-      <c r="I52">
-        <v>11706</v>
+        <v>1435307</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>23570892</v>
-      </c>
-      <c r="B53">
-        <v>28168</v>
+        <v>23570893</v>
+      </c>
+      <c r="B53" s="1">
+        <f>(((A53)/60)/24)+DATE(1970,1,1)</f>
+        <v>41937.675694444442</v>
       </c>
       <c r="C53">
-        <v>11706</v>
-      </c>
-      <c r="E53" s="1">
-        <f>(((A54)/60)/24)+DATE(1970,1,1)</f>
-        <v>41937.675694444442</v>
+        <v>18247</v>
+      </c>
+      <c r="D53" s="2">
+        <v>36.352583459151099</v>
+      </c>
+      <c r="E53">
+        <v>23844</v>
       </c>
       <c r="F53">
-        <v>18247</v>
-      </c>
-      <c r="G53" s="2">
-        <v>36.352583459151099</v>
+        <v>9737</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>866790.99999999884</v>
       </c>
       <c r="H53">
-        <v>23844</v>
-      </c>
-      <c r="I53">
-        <v>9737</v>
+        <v>866791</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>23570893</v>
-      </c>
-      <c r="B54">
-        <v>23844</v>
-      </c>
-      <c r="C54">
-        <v>9737</v>
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E55">
+        <f>SUM(E2:E53)</f>
+        <v>2350539</v>
+      </c>
+      <c r="G55" s="2">
+        <f>SUM(G2:G53)</f>
+        <v>140332530.99999994</v>
+      </c>
+      <c r="H55" s="2">
+        <f>SUM(H2:H53)</f>
+        <v>140332531</v>
+      </c>
+      <c r="I55" s="2">
+        <f>G55-H55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <f>H55/E55</f>
+        <v>59.702277222373255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Präsentation überarbeitet, Messung für Single-Core optimiert
</commit_message>
<xml_diff>
--- a/Auswertung.xlsx
+++ b/Auswertung.xlsx
@@ -48,12 +48,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Anz. Res_send</t>
-  </si>
-  <si>
-    <t>Average Duration</t>
-  </si>
-  <si>
     <t>Anzahl client events</t>
   </si>
   <si>
@@ -73,6 +67,12 @@
   </si>
   <si>
     <t>Durchschnittliche Dauer eine Client-Requests:</t>
+  </si>
+  <si>
+    <t>Task 1: Anz. Res_send / Minute</t>
+  </si>
+  <si>
+    <t>Task 2: Average Duration</t>
   </si>
 </sst>
 </file>
@@ -503,11 +503,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="230764544"/>
-        <c:axId val="230766080"/>
+        <c:axId val="239218688"/>
+        <c:axId val="239220224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="230764544"/>
+        <c:axId val="239218688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -517,7 +517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="230766080"/>
+        <c:crossAx val="239220224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -525,7 +525,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="230766080"/>
+        <c:axId val="239220224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,7 +536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="230764544"/>
+        <c:crossAx val="239218688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -581,7 +581,7 @@
           <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Anzahl Nachrichten &amp; Antworten Client</c:v>
+            <c:v>Task 1: Anzahl res_snd pro Minute, Server-Log (Anzahl Calls)</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -912,688 +912,6 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>23844</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Anzahl Fehler Client</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Tabelle2!$B$2:$B$53</c:f>
-              <c:numCache>
-                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>41937.640277777777</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41937.640972222223</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41937.64166666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41937.642361111109</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41937.643055555556</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41937.643750000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41937.644444444442</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41937.645138888889</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41937.645833333336</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41937.646527777775</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41937.647222222222</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41937.647916666669</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41937.648611111108</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41937.649305555555</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41937.65</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41937.650694444441</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>41937.651388888888</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>41937.652083333334</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>41937.652777777781</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>41937.65347222222</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>41937.654166666667</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>41937.654861111114</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>41937.655555555553</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>41937.65625</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>41937.656944444447</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>41937.657638888886</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>41937.658333333333</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>41937.65902777778</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>41937.659722222219</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>41937.660416666666</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>41937.661111111112</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>41937.661805555559</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>41937.662499999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>41937.663194444445</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>41937.663888888892</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>41937.664583333331</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>41937.665277777778</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>41937.665972222225</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>41937.666666666664</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>41937.667361111111</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41937.668055555558</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>41937.668749999997</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>41937.669444444444</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>41937.670138888891</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>41937.67083333333</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>41937.671527777777</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>41937.672222222223</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>41937.67291666667</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>41937.673611111109</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>41937.674305555556</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>41937.675000000003</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>41937.675694444442</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle2!$F$2:$F$53</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>33366</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30183</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32545</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32933</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>32814</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>31620</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30257</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>27481</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>25055</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>24247</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>23873</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>23346</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>22616</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>22196</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>21171</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>20731</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>20153</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>20267</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19842</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>18841</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>18990</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>18519</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>18297</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>17905</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>17851</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>17418</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>16993</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>16635</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>16288</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>16335</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>16061</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>15884</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>15748</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>14650</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>14631</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>14749</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>14486</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>14899</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>14088</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>14120</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>14225</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>14068</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>13558</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>13324</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>13042</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>13004</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>12951</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>12941</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>12187</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>11418</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>11706</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>9737</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Anzahl res_send Server</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Tabelle2!$B$2:$B$53</c:f>
-              <c:numCache>
-                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>41937.640277777777</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41937.640972222223</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41937.64166666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41937.642361111109</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41937.643055555556</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41937.643750000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41937.644444444442</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41937.645138888889</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41937.645833333336</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41937.646527777775</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41937.647222222222</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41937.647916666669</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41937.648611111108</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41937.649305555555</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41937.65</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41937.650694444441</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>41937.651388888888</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>41937.652083333334</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>41937.652777777781</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>41937.65347222222</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>41937.654166666667</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>41937.654861111114</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>41937.655555555553</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>41937.65625</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>41937.656944444447</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>41937.657638888886</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>41937.658333333333</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>41937.65902777778</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>41937.659722222219</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>41937.660416666666</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>41937.661111111112</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>41937.661805555559</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>41937.662499999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>41937.663194444445</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>41937.663888888892</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>41937.664583333331</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>41937.665277777778</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>41937.665972222225</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>41937.666666666664</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>41937.667361111111</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41937.668055555558</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>41937.668749999997</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>41937.669444444444</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>41937.670138888891</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>41937.67083333333</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>41937.671527777777</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>41937.672222222223</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>41937.67291666667</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>41937.673611111109</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>41937.674305555556</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>41937.675000000003</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>41937.675694444442</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle2!$C$2:$C$53</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>25669</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>22612</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>23366</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22102</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21049</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19422</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>18125</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16722</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14897</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14461</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14214</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13707</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13431</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13228</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>12647</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>12479</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>12028</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>12043</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>11723</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>11232</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>11341</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>11029</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11030</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>10764</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>10815</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>10390</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>10292</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>10189</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9877</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>10010</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>9805</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9768</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9556</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>8995</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>9002</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>9151</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>8995</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9032</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>8819</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>8755</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>8707</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>8687</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>8458</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>8463</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>8218</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>8374</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>8261</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>8096</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>11708</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>14966</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>15136</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>18247</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1610,17 +928,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="231446400"/>
-        <c:axId val="231447936"/>
+        <c:axId val="240494464"/>
+        <c:axId val="240496000"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
-            <c:v>Durchschnittliche Dauer (Sekunden)</c:v>
+            <c:v>Task 2: Mittlere Response_Time pro Minute (Sekunden)</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -1967,11 +1285,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="231459456"/>
-        <c:axId val="231457920"/>
+        <c:axId val="240507520"/>
+        <c:axId val="240505984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="231446400"/>
+        <c:axId val="240494464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1981,7 +1299,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="231447936"/>
+        <c:crossAx val="240496000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1989,7 +1307,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="231447936"/>
+        <c:axId val="240496000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2000,12 +1318,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="231446400"/>
+        <c:crossAx val="240494464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="231457920"/>
+        <c:axId val="240505984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2015,12 +1333,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="231459456"/>
+        <c:crossAx val="240507520"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="231459456"/>
+        <c:axId val="240507520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2030,7 +1348,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="231457920"/>
+        <c:crossAx val="240505984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3068,18 +2386,19 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="0.44140625" customWidth="1"/>
+    <col min="8" max="8" width="0.77734375" customWidth="1"/>
     <col min="9" max="9" width="18.6640625" customWidth="1"/>
     <col min="10" max="10" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.21875" bestFit="1" customWidth="1"/>
@@ -3087,28 +2406,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3116,7 +2435,7 @@
         <v>23570842</v>
       </c>
       <c r="B2" s="1">
-        <f>(((A2)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" ref="B2:B33" si="0">(((A2)/60)/24)+DATE(1970,1,1)</f>
         <v>41937.640277777777</v>
       </c>
       <c r="C2">
@@ -3144,7 +2463,7 @@
         <v>23570843</v>
       </c>
       <c r="B3" s="1">
-        <f>(((A3)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.640972222223</v>
       </c>
       <c r="C3">
@@ -3160,7 +2479,7 @@
         <v>30183</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G53" si="0">D3*E3</f>
+        <f t="shared" ref="G3:G53" si="1">D3*E3</f>
         <v>2815943.9999999935</v>
       </c>
       <c r="H3">
@@ -3172,7 +2491,7 @@
         <v>23570844</v>
       </c>
       <c r="B4" s="1">
-        <f>(((A4)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.64166666667</v>
       </c>
       <c r="C4">
@@ -3188,7 +2507,7 @@
         <v>32545</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816710.9999999977</v>
       </c>
       <c r="H4">
@@ -3200,7 +2519,7 @@
         <v>23570845</v>
       </c>
       <c r="B5" s="1">
-        <f>(((A5)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.642361111109</v>
       </c>
       <c r="C5">
@@ -3216,7 +2535,7 @@
         <v>32933</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816311.9999999958</v>
       </c>
       <c r="H5">
@@ -3228,7 +2547,7 @@
         <v>23570846</v>
       </c>
       <c r="B6" s="1">
-        <f>(((A6)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.643055555556</v>
       </c>
       <c r="C6">
@@ -3244,7 +2563,7 @@
         <v>32814</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816094.9999999972</v>
       </c>
       <c r="H6">
@@ -3256,7 +2575,7 @@
         <v>23570847</v>
       </c>
       <c r="B7" s="1">
-        <f>(((A7)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.643750000003</v>
       </c>
       <c r="C7">
@@ -3272,7 +2591,7 @@
         <v>31620</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817495.9999999944</v>
       </c>
       <c r="H7">
@@ -3284,7 +2603,7 @@
         <v>23570848</v>
       </c>
       <c r="B8" s="1">
-        <f>(((A8)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.644444444442</v>
       </c>
       <c r="C8">
@@ -3300,7 +2619,7 @@
         <v>30257</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2815971.9999999995</v>
       </c>
       <c r="H8">
@@ -3312,7 +2631,7 @@
         <v>23570849</v>
       </c>
       <c r="B9" s="1">
-        <f>(((A9)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.645138888889</v>
       </c>
       <c r="C9">
@@ -3328,7 +2647,7 @@
         <v>27481</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2818491.9999999958</v>
       </c>
       <c r="H9">
@@ -3340,7 +2659,7 @@
         <v>23570850</v>
       </c>
       <c r="B10" s="1">
-        <f>(((A10)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.645833333336</v>
       </c>
       <c r="C10">
@@ -3356,7 +2675,7 @@
         <v>25055</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816342</v>
       </c>
       <c r="H10">
@@ -3368,7 +2687,7 @@
         <v>23570851</v>
       </c>
       <c r="B11" s="1">
-        <f>(((A11)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.646527777775</v>
       </c>
       <c r="C11">
@@ -3384,7 +2703,7 @@
         <v>24247</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816761</v>
       </c>
       <c r="H11">
@@ -3396,7 +2715,7 @@
         <v>23570852</v>
       </c>
       <c r="B12" s="1">
-        <f>(((A12)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.647222222222</v>
       </c>
       <c r="C12">
@@ -3412,7 +2731,7 @@
         <v>23873</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817747.9999999977</v>
       </c>
       <c r="H12">
@@ -3424,7 +2743,7 @@
         <v>23570853</v>
       </c>
       <c r="B13" s="1">
-        <f>(((A13)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.647916666669</v>
       </c>
       <c r="C13">
@@ -3440,7 +2759,7 @@
         <v>23346</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817756.9999999986</v>
       </c>
       <c r="H13">
@@ -3452,7 +2771,7 @@
         <v>23570854</v>
       </c>
       <c r="B14" s="1">
-        <f>(((A14)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.648611111108</v>
       </c>
       <c r="C14">
@@ -3468,7 +2787,7 @@
         <v>22616</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2818738</v>
       </c>
       <c r="H14">
@@ -3480,7 +2799,7 @@
         <v>23570855</v>
       </c>
       <c r="B15" s="1">
-        <f>(((A15)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.649305555555</v>
       </c>
       <c r="C15">
@@ -3496,7 +2815,7 @@
         <v>22196</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816372.9999999953</v>
       </c>
       <c r="H15">
@@ -3508,7 +2827,7 @@
         <v>23570856</v>
       </c>
       <c r="B16" s="1">
-        <f>(((A16)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.65</v>
       </c>
       <c r="C16">
@@ -3524,7 +2843,7 @@
         <v>21171</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2818901.9999999977</v>
       </c>
       <c r="H16">
@@ -3536,7 +2855,7 @@
         <v>23570857</v>
       </c>
       <c r="B17" s="1">
-        <f>(((A17)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.650694444441</v>
       </c>
       <c r="C17">
@@ -3552,7 +2871,7 @@
         <v>20731</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2815453.9999999958</v>
       </c>
       <c r="H17">
@@ -3564,7 +2883,7 @@
         <v>23570858</v>
       </c>
       <c r="B18" s="1">
-        <f>(((A18)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.651388888888</v>
       </c>
       <c r="C18">
@@ -3580,7 +2899,7 @@
         <v>20153</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817974.9999999958</v>
       </c>
       <c r="H18">
@@ -3592,7 +2911,7 @@
         <v>23570859</v>
       </c>
       <c r="B19" s="1">
-        <f>(((A19)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.652083333334</v>
       </c>
       <c r="C19">
@@ -3608,7 +2927,7 @@
         <v>20267</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817965.9999999991</v>
       </c>
       <c r="H19">
@@ -3620,7 +2939,7 @@
         <v>23570860</v>
       </c>
       <c r="B20" s="1">
-        <f>(((A20)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.652777777781</v>
       </c>
       <c r="C20">
@@ -3636,7 +2955,7 @@
         <v>19842</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816115.9999999991</v>
       </c>
       <c r="H20">
@@ -3648,7 +2967,7 @@
         <v>23570861</v>
       </c>
       <c r="B21" s="1">
-        <f>(((A21)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.65347222222</v>
       </c>
       <c r="C21">
@@ -3664,7 +2983,7 @@
         <v>18841</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817915</v>
       </c>
       <c r="H21">
@@ -3676,7 +2995,7 @@
         <v>23570862</v>
       </c>
       <c r="B22" s="1">
-        <f>(((A22)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.654166666667</v>
       </c>
       <c r="C22">
@@ -3692,7 +3011,7 @@
         <v>18990</v>
       </c>
       <c r="G22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816655.9999999977</v>
       </c>
       <c r="H22">
@@ -3704,7 +3023,7 @@
         <v>23570863</v>
       </c>
       <c r="B23" s="1">
-        <f>(((A23)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.654861111114</v>
       </c>
       <c r="C23">
@@ -3720,7 +3039,7 @@
         <v>18519</v>
       </c>
       <c r="G23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2818614.9999999972</v>
       </c>
       <c r="H23">
@@ -3732,7 +3051,7 @@
         <v>23570864</v>
       </c>
       <c r="B24" s="1">
-        <f>(((A24)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.655555555553</v>
       </c>
       <c r="C24">
@@ -3748,7 +3067,7 @@
         <v>18297</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816787</v>
       </c>
       <c r="H24">
@@ -3760,7 +3079,7 @@
         <v>23570865</v>
       </c>
       <c r="B25" s="1">
-        <f>(((A25)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.65625</v>
       </c>
       <c r="C25">
@@ -3776,7 +3095,7 @@
         <v>17905</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817676.9999999967</v>
       </c>
       <c r="H25">
@@ -3788,7 +3107,7 @@
         <v>23570866</v>
       </c>
       <c r="B26" s="1">
-        <f>(((A26)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.656944444447</v>
       </c>
       <c r="C26">
@@ -3804,7 +3123,7 @@
         <v>17851</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2815771.9999999981</v>
       </c>
       <c r="H26">
@@ -3816,7 +3135,7 @@
         <v>23570867</v>
       </c>
       <c r="B27" s="1">
-        <f>(((A27)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.657638888886</v>
       </c>
       <c r="C27">
@@ -3832,7 +3151,7 @@
         <v>17418</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2818798.9999999977</v>
       </c>
       <c r="H27">
@@ -3844,7 +3163,7 @@
         <v>23570868</v>
       </c>
       <c r="B28" s="1">
-        <f>(((A28)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.658333333333</v>
       </c>
       <c r="C28">
@@ -3860,7 +3179,7 @@
         <v>16993</v>
       </c>
       <c r="G28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816314.9999999963</v>
       </c>
       <c r="H28">
@@ -3872,7 +3191,7 @@
         <v>23570869</v>
       </c>
       <c r="B29" s="1">
-        <f>(((A29)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.65902777778</v>
       </c>
       <c r="C29">
@@ -3888,7 +3207,7 @@
         <v>16635</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817421.9999999986</v>
       </c>
       <c r="H29">
@@ -3900,7 +3219,7 @@
         <v>23570870</v>
       </c>
       <c r="B30" s="1">
-        <f>(((A30)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.659722222219</v>
       </c>
       <c r="C30">
@@ -3916,7 +3235,7 @@
         <v>16288</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817586.9999999967</v>
       </c>
       <c r="H30">
@@ -3928,7 +3247,7 @@
         <v>23570871</v>
       </c>
       <c r="B31" s="1">
-        <f>(((A31)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.660416666666</v>
       </c>
       <c r="C31">
@@ -3944,7 +3263,7 @@
         <v>16335</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2819319</v>
       </c>
       <c r="H31">
@@ -3956,7 +3275,7 @@
         <v>23570872</v>
       </c>
       <c r="B32" s="1">
-        <f>(((A32)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.661111111112</v>
       </c>
       <c r="C32">
@@ -3972,7 +3291,7 @@
         <v>16061</v>
       </c>
       <c r="G32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816992.9999999967</v>
       </c>
       <c r="H32">
@@ -3984,7 +3303,7 @@
         <v>23570873</v>
       </c>
       <c r="B33" s="1">
-        <f>(((A33)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="0"/>
         <v>41937.661805555559</v>
       </c>
       <c r="C33">
@@ -4000,7 +3319,7 @@
         <v>15884</v>
       </c>
       <c r="G33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817149.9999999972</v>
       </c>
       <c r="H33">
@@ -4012,7 +3331,7 @@
         <v>23570874</v>
       </c>
       <c r="B34" s="1">
-        <f>(((A34)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" ref="B34:B65" si="2">(((A34)/60)/24)+DATE(1970,1,1)</f>
         <v>41937.662499999999</v>
       </c>
       <c r="C34">
@@ -4028,7 +3347,7 @@
         <v>15748</v>
       </c>
       <c r="G34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817098.9999999986</v>
       </c>
       <c r="H34">
@@ -4040,7 +3359,7 @@
         <v>23570875</v>
       </c>
       <c r="B35" s="1">
-        <f>(((A35)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.663194444445</v>
       </c>
       <c r="C35">
@@ -4056,7 +3375,7 @@
         <v>14650</v>
       </c>
       <c r="G35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2820018.9999999967</v>
       </c>
       <c r="H35">
@@ -4068,7 +3387,7 @@
         <v>23570876</v>
       </c>
       <c r="B36" s="1">
-        <f>(((A36)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.663888888892</v>
       </c>
       <c r="C36">
@@ -4084,7 +3403,7 @@
         <v>14631</v>
       </c>
       <c r="G36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816389.9999999972</v>
       </c>
       <c r="H36">
@@ -4096,7 +3415,7 @@
         <v>23570877</v>
       </c>
       <c r="B37" s="1">
-        <f>(((A37)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.664583333331</v>
       </c>
       <c r="C37">
@@ -4112,7 +3431,7 @@
         <v>14749</v>
       </c>
       <c r="G37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2818884.9999999995</v>
       </c>
       <c r="H37">
@@ -4124,7 +3443,7 @@
         <v>23570878</v>
       </c>
       <c r="B38" s="1">
-        <f>(((A38)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.665277777778</v>
       </c>
       <c r="C38">
@@ -4140,7 +3459,7 @@
         <v>14486</v>
       </c>
       <c r="G38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816044.9999999977</v>
       </c>
       <c r="H38">
@@ -4152,7 +3471,7 @@
         <v>23570879</v>
       </c>
       <c r="B39" s="1">
-        <f>(((A39)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.665972222225</v>
       </c>
       <c r="C39">
@@ -4168,7 +3487,7 @@
         <v>14899</v>
       </c>
       <c r="G39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2818846.9999999981</v>
       </c>
       <c r="H39">
@@ -4180,7 +3499,7 @@
         <v>23570880</v>
       </c>
       <c r="B40" s="1">
-        <f>(((A40)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.666666666664</v>
       </c>
       <c r="C40">
@@ -4196,7 +3515,7 @@
         <v>14088</v>
       </c>
       <c r="G40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2816719.9999999986</v>
       </c>
       <c r="H40">
@@ -4208,7 +3527,7 @@
         <v>23570881</v>
       </c>
       <c r="B41" s="1">
-        <f>(((A41)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.667361111111</v>
       </c>
       <c r="C41">
@@ -4224,7 +3543,7 @@
         <v>14120</v>
       </c>
       <c r="G41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2819099.9999999995</v>
       </c>
       <c r="H41">
@@ -4236,7 +3555,7 @@
         <v>23570882</v>
       </c>
       <c r="B42" s="1">
-        <f>(((A42)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.668055555558</v>
       </c>
       <c r="C42">
@@ -4252,7 +3571,7 @@
         <v>14225</v>
       </c>
       <c r="G42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2815940.9999999995</v>
       </c>
       <c r="H42">
@@ -4264,7 +3583,7 @@
         <v>23570883</v>
       </c>
       <c r="B43" s="1">
-        <f>(((A43)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.668749999997</v>
       </c>
       <c r="C43">
@@ -4280,7 +3599,7 @@
         <v>14068</v>
       </c>
       <c r="G43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2819621.9999999977</v>
       </c>
       <c r="H43">
@@ -4292,7 +3611,7 @@
         <v>23570884</v>
       </c>
       <c r="B44" s="1">
-        <f>(((A44)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.669444444444</v>
       </c>
       <c r="C44">
@@ -4308,7 +3627,7 @@
         <v>13558</v>
       </c>
       <c r="G44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2815278</v>
       </c>
       <c r="H44">
@@ -4320,7 +3639,7 @@
         <v>23570885</v>
       </c>
       <c r="B45" s="1">
-        <f>(((A45)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.670138888891</v>
       </c>
       <c r="C45">
@@ -4336,7 +3655,7 @@
         <v>13324</v>
       </c>
       <c r="G45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2822889.9999999977</v>
       </c>
       <c r="H45">
@@ -4348,7 +3667,7 @@
         <v>23570886</v>
       </c>
       <c r="B46" s="1">
-        <f>(((A46)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.67083333333</v>
       </c>
       <c r="C46">
@@ -4364,7 +3683,7 @@
         <v>13042</v>
       </c>
       <c r="G46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2815064.9999999991</v>
       </c>
       <c r="H46">
@@ -4376,7 +3695,7 @@
         <v>23570887</v>
       </c>
       <c r="B47" s="1">
-        <f>(((A47)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.671527777777</v>
       </c>
       <c r="C47">
@@ -4392,7 +3711,7 @@
         <v>13004</v>
       </c>
       <c r="G47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2817494.9999999972</v>
       </c>
       <c r="H47">
@@ -4404,7 +3723,7 @@
         <v>23570888</v>
       </c>
       <c r="B48" s="1">
-        <f>(((A48)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.672222222223</v>
       </c>
       <c r="C48">
@@ -4420,7 +3739,7 @@
         <v>12951</v>
       </c>
       <c r="G48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2821606.9999999981</v>
       </c>
       <c r="H48">
@@ -4432,7 +3751,7 @@
         <v>23570889</v>
       </c>
       <c r="B49" s="1">
-        <f>(((A49)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.67291666667</v>
       </c>
       <c r="C49">
@@ -4448,7 +3767,7 @@
         <v>12941</v>
       </c>
       <c r="G49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2756663.9999999986</v>
       </c>
       <c r="H49">
@@ -4460,7 +3779,7 @@
         <v>23570890</v>
       </c>
       <c r="B50" s="1">
-        <f>(((A50)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.673611111109</v>
       </c>
       <c r="C50">
@@ -4476,7 +3795,7 @@
         <v>12187</v>
       </c>
       <c r="G50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1805459.9999999988</v>
       </c>
       <c r="H50">
@@ -4488,7 +3807,7 @@
         <v>23570891</v>
       </c>
       <c r="B51" s="1">
-        <f>(((A51)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.674305555556</v>
       </c>
       <c r="C51">
@@ -4504,7 +3823,7 @@
         <v>11418</v>
       </c>
       <c r="G51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1439369.9999999979</v>
       </c>
       <c r="H51">
@@ -4516,7 +3835,7 @@
         <v>23570892</v>
       </c>
       <c r="B52" s="1">
-        <f>(((A52)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.675000000003</v>
       </c>
       <c r="C52">
@@ -4532,7 +3851,7 @@
         <v>11706</v>
       </c>
       <c r="G52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1435306.9999999977</v>
       </c>
       <c r="H52">
@@ -4544,7 +3863,7 @@
         <v>23570893</v>
       </c>
       <c r="B53" s="1">
-        <f>(((A53)/60)/24)+DATE(1970,1,1)</f>
+        <f t="shared" si="2"/>
         <v>41937.675694444442</v>
       </c>
       <c r="C53">
@@ -4560,7 +3879,7 @@
         <v>9737</v>
       </c>
       <c r="G53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>866790.99999999884</v>
       </c>
       <c r="H53">
@@ -4569,7 +3888,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E54" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -4592,7 +3911,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G57" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>